<commit_message>
DCF Update for NorwegianCruiseLineHoldings (NCLH)
Undervalued, but seemingly very risky play. More DD required.
Price target: $26.17
</commit_message>
<xml_diff>
--- a/DCF Models/NCLH.xlsx
+++ b/DCF Models/NCLH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\DCF Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F001F8D-72B3-4DD4-8815-EA9126ABDDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C58025-0EC9-4F4A-AFF5-58D967EA9C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="3195" windowWidth="32700" windowHeight="15045" xr2:uid="{3056AFBF-C33C-44A0-B793-E31A92920761}"/>
+    <workbookView xWindow="5835" yWindow="5055" windowWidth="27045" windowHeight="15045" activeTab="1" xr2:uid="{3056AFBF-C33C-44A0-B793-E31A92920761}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="86">
   <si>
     <t>Price</t>
   </si>
@@ -236,9 +236,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Remainder of 2022</t>
-  </si>
-  <si>
     <t>$</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t>Extras per APCD</t>
+  </si>
+  <si>
+    <t>25% was variable debt</t>
   </si>
 </sst>
 </file>
@@ -443,14 +443,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
@@ -467,8 +467,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14801850" y="0"/>
-          <a:ext cx="0" cy="10601325"/>
+          <a:off x="17840325" y="0"/>
+          <a:ext cx="0" cy="11553825"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -843,8 +843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B3E6B5-2ED0-4ACF-895E-E286D10A7127}">
   <dimension ref="B2:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +857,7 @@
         <v>7</v>
       </c>
       <c r="N2" s="1">
-        <v>44972</v>
+        <v>44985</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
@@ -865,7 +865,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="2">
-        <v>18.11</v>
+        <v>14.56</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -882,7 +882,7 @@
       </c>
       <c r="N6" s="4">
         <f>N4*N5</f>
-        <v>6618.2813900000001</v>
+        <v>5320.9374400000006</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
@@ -890,7 +890,7 @@
         <v>3</v>
       </c>
       <c r="N7" s="4">
-        <v>1186.7</v>
+        <v>946.98699999999997</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
@@ -898,8 +898,7 @@
         <v>4</v>
       </c>
       <c r="N8" s="4">
-        <f>1012.7+141.3+12893.407</f>
-        <v>14047.406999999999</v>
+        <v>13850.27</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
@@ -908,7 +907,7 @@
       </c>
       <c r="N9" s="4">
         <f>+N6-N7+N8</f>
-        <v>19478.988389999999</v>
+        <v>18224.220440000001</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
@@ -925,7 +924,7 @@
       </c>
       <c r="N12" s="4">
         <f>Dash!C4</f>
-        <v>9576.3280554549001</v>
+        <v>9564.1035156825055</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
@@ -934,12 +933,12 @@
       </c>
       <c r="N13" s="2">
         <f>N12/N5</f>
-        <v>26.204280365946822</v>
+        <v>26.170829625152908</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
@@ -959,7 +958,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -974,91 +973,86 @@
       </c>
       <c r="E21" s="25"/>
     </row>
-    <row r="22" spans="2:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="16">
+        <v>2023</v>
+      </c>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="15">
+        <v>988.072</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="12">
+        <v>2024</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="19">
+        <v>2510.4630000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="16">
+        <v>2025</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="15">
+        <v>2433.0010000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="12">
+        <v>2026</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="19">
+        <v>2047.2750000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="16">
+        <v>2027</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="19">
+        <v>3099.8679999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="21">
+        <f>13839.885-SUM(E22:E26)</f>
+        <v>2761.2060000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="15">
-        <v>332696</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="16">
-        <v>2023</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19">
-        <v>1001343</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="12">
-        <v>2024</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15">
-        <v>3763958</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="16">
-        <v>2025</v>
-      </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="19">
-        <v>1148007</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="12">
-        <v>2026</v>
-      </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15">
-        <v>2050992</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="16">
-        <v>2027</v>
-      </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="19">
-        <v>3101980</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21">
-        <v>2753755</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="23">
-        <v>14152731</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E28" s="23">
+        <f>SUM(E22:E27)</f>
+        <v>13839.885</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D21:E21"/>
@@ -1071,11 +1065,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44922598-A76D-432E-8D6B-EF22B15EDFE4}">
   <dimension ref="A2:DX82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="N48" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S5" sqref="S5"/>
+      <selection pane="bottomRight" activeCell="AO8" sqref="AO8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,6 +1471,10 @@
       <c r="I3" s="4">
         <v>1105.9000000000001</v>
       </c>
+      <c r="J3" s="4">
+        <f>+AA3-I3-H3-G3</f>
+        <v>1011.5530000000001</v>
+      </c>
       <c r="O3" s="4">
         <v>1411.8</v>
       </c>
@@ -1514,8 +1512,7 @@
         <v>392.75200000000001</v>
       </c>
       <c r="AA3" s="4">
-        <f>G3+H3+I3+I3</f>
-        <v>3348.1470000000004</v>
+        <v>3253.8</v>
       </c>
     </row>
     <row r="4" spans="2:128" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1544,6 +1541,10 @@
       <c r="I4" s="4">
         <v>509.6</v>
       </c>
+      <c r="J4" s="4">
+        <f>+AA4-I4-H4-G4</f>
+        <v>507.56000000000017</v>
+      </c>
       <c r="O4" s="4">
         <v>600.29999999999995</v>
       </c>
@@ -1581,8 +1582,7 @@
         <v>255.23</v>
       </c>
       <c r="AA4" s="4">
-        <f>G4+H4+I4+I4</f>
-        <v>1592</v>
+        <v>1589.96</v>
       </c>
     </row>
     <row r="5" spans="2:128" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="J5" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1519.1130000000003</v>
       </c>
       <c r="O5" s="5">
         <f>+O3+O4</f>
@@ -1671,15 +1671,15 @@
       </c>
       <c r="AA5" s="5">
         <f t="shared" si="1"/>
-        <v>4940.1470000000008</v>
+        <v>4843.76</v>
       </c>
       <c r="AB5" s="5">
         <f>AA5+(-$AA$5+$AD$5)/3</f>
-        <v>5977.4103737637524</v>
+        <v>5913.1523737637517</v>
       </c>
       <c r="AC5" s="5">
         <f>AB5+(-$AA$5+$AD$5)/3</f>
-        <v>7014.673747527504</v>
+        <v>6982.5447475275032</v>
       </c>
       <c r="AD5" s="5">
         <f>X5*(1+Y62)*(1+Z62)*(1+AA62)*(1+AB62)*(1+AC62)*(1+AD62)</f>
@@ -1740,6 +1740,10 @@
       <c r="I6" s="4">
         <v>352.8</v>
       </c>
+      <c r="J6" s="4">
+        <f t="shared" ref="J6:J11" si="4">+AA6-I6-H6-G6</f>
+        <v>337.67200000000014</v>
+      </c>
       <c r="S6" s="4">
         <v>503.72199999999998</v>
       </c>
@@ -1765,12 +1769,11 @@
         <v>143.524</v>
       </c>
       <c r="AA6" s="4">
-        <f t="shared" ref="AA6:AA11" si="4">G6+H6+I6+I6</f>
-        <v>1049.758</v>
+        <v>1034.6300000000001</v>
       </c>
       <c r="AB6" s="4">
         <f>AC6/2+AA6/2</f>
-        <v>1204.8248272524147</v>
+        <v>1197.2608272524149</v>
       </c>
       <c r="AC6" s="4">
         <f>X6*(1+Y62)*(1+Z62)*(1+AA62)*(1+AB62)*(1+AC62)</f>
@@ -1835,6 +1838,10 @@
       <c r="I7" s="4">
         <v>126.74</v>
       </c>
+      <c r="J7" s="4">
+        <f t="shared" si="4"/>
+        <v>102.485</v>
+      </c>
       <c r="S7" s="4">
         <v>224</v>
       </c>
@@ -1860,12 +1867,11 @@
         <v>54.03</v>
       </c>
       <c r="AA7" s="4">
-        <f t="shared" si="4"/>
-        <v>382.185</v>
+        <v>357.93</v>
       </c>
       <c r="AB7" s="4">
         <f>AC7/2+AA7/2</f>
-        <v>430.5202973204818</v>
+        <v>418.3927973204818</v>
       </c>
       <c r="AC7" s="4">
         <f>X7*(1+Y62)*(1+Z62)*(1+AA62)*(1+AB62)*(1+AC62)</f>
@@ -1930,6 +1936,10 @@
       <c r="I8" s="4">
         <v>287.39999999999998</v>
       </c>
+      <c r="J8" s="4">
+        <f t="shared" si="4"/>
+        <v>297.91300000000012</v>
+      </c>
       <c r="S8" s="4">
         <v>452.65</v>
       </c>
@@ -1955,12 +1965,11 @@
         <v>537.44000000000005</v>
       </c>
       <c r="AA8" s="4">
-        <f t="shared" si="4"/>
-        <v>1078.127</v>
+        <v>1088.6400000000001</v>
       </c>
       <c r="AB8" s="4">
         <f>AC8/2+AA8/2</f>
-        <v>1147.9241882822189</v>
+        <v>1153.1806882822191</v>
       </c>
       <c r="AC8" s="4">
         <f>X8*(1+Y55)*(1+Z55)*(1+AA55)*(1+AB55)*(1+AC55)</f>
@@ -2025,6 +2034,10 @@
       <c r="I9" s="4">
         <v>186.98400000000001</v>
       </c>
+      <c r="J9" s="4">
+        <f t="shared" si="4"/>
+        <v>183.14100000000002</v>
+      </c>
       <c r="S9" s="4">
         <v>326.23</v>
       </c>
@@ -2050,8 +2063,7 @@
         <v>301.85000000000002</v>
       </c>
       <c r="AA9" s="4">
-        <f t="shared" si="4"/>
-        <v>690.66800000000001</v>
+        <v>686.82500000000005</v>
       </c>
       <c r="AB9" s="4">
         <f>X9*(1+Y58)*(1+Z58)*(1+AA58)*(1+AB58)</f>
@@ -2120,6 +2132,10 @@
       <c r="I10" s="4">
         <v>76.81</v>
       </c>
+      <c r="J10" s="4">
+        <f t="shared" si="4"/>
+        <v>86.274000000000001</v>
+      </c>
       <c r="S10" s="4">
         <v>168.24</v>
       </c>
@@ -2145,12 +2161,11 @@
         <v>63</v>
       </c>
       <c r="AA10" s="4">
-        <f t="shared" si="4"/>
-        <v>254.33600000000001</v>
+        <v>263.8</v>
       </c>
       <c r="AB10" s="4">
         <f>AC10/2+AA10/2</f>
-        <v>275.0814516653947</v>
+        <v>279.81345166539472</v>
       </c>
       <c r="AC10" s="4">
         <f>X10*(1+Y60)*(1+Z60)*(1+AA60)*(1+AB60)*(1+AC60)</f>
@@ -2215,6 +2230,10 @@
       <c r="I11" s="4">
         <v>208.17599999999999</v>
       </c>
+      <c r="J11" s="4">
+        <f t="shared" si="4"/>
+        <v>211.87550000000007</v>
+      </c>
       <c r="S11" s="4">
         <v>271.8</v>
       </c>
@@ -2240,12 +2259,11 @@
         <v>508.18599999999998</v>
       </c>
       <c r="AA11" s="4">
-        <f t="shared" si="4"/>
-        <v>831.55049999999983</v>
+        <v>835.25</v>
       </c>
       <c r="AB11" s="4">
         <f>AC11/2+AA11/2</f>
-        <v>774.48625498478248</v>
+        <v>776.33600498478256</v>
       </c>
       <c r="AC11" s="4">
         <f>X11*(1+Y62)*(1+Z62)*(1+AA62)*(1+AB62)*(1+AC62)</f>
@@ -2318,7 +2336,7 @@
       </c>
       <c r="J12" s="4">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1219.3605000000002</v>
       </c>
       <c r="S12" s="4">
         <f t="shared" ref="S12:AC12" si="12">+S6+S7+S8+S9+S10+S11</f>
@@ -2354,11 +2372,11 @@
       </c>
       <c r="AA12" s="4">
         <f>+AA6+AA7+AA8+AA9+AA10+AA11</f>
-        <v>4286.6244999999999</v>
+        <v>4267.0750000000007</v>
       </c>
       <c r="AB12" s="4">
         <f>+AB6+AB7+AB8+AB9+AB10+AB11</f>
-        <v>4435.1899606817633</v>
+        <v>4427.3367106817641</v>
       </c>
       <c r="AC12" s="4">
         <f t="shared" si="12"/>
@@ -2431,7 +2449,7 @@
       </c>
       <c r="J13" s="5">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>299.75250000000005</v>
       </c>
       <c r="S13" s="5">
         <f t="shared" ref="S13:AA13" si="15">+S5-S12</f>
@@ -2467,15 +2485,15 @@
       </c>
       <c r="AA13" s="5">
         <f t="shared" si="15"/>
-        <v>653.52250000000095</v>
+        <v>576.68499999999949</v>
       </c>
       <c r="AB13" s="5">
         <f t="shared" ref="AB13:AK13" si="16">+AB5-AB12</f>
-        <v>1542.2204130819891</v>
+        <v>1485.8156630819876</v>
       </c>
       <c r="AC13" s="5">
         <f>+AC5-AC12</f>
-        <v>2390.7915026345654</v>
+        <v>2358.6625026345646</v>
       </c>
       <c r="AD13" s="5">
         <f>+AD5-AD12</f>
@@ -2536,6 +2554,10 @@
       <c r="I14" s="4">
         <v>375.29</v>
       </c>
+      <c r="J14" s="4">
+        <f t="shared" ref="J14:J16" si="17">+AA14-I14-H14-G14</f>
+        <v>378.52800000000013</v>
+      </c>
       <c r="S14" s="4">
         <v>403.17</v>
       </c>
@@ -2561,47 +2583,46 @@
         <v>891.45</v>
       </c>
       <c r="AA14" s="4">
-        <f>G14+H14+I14+I14</f>
-        <v>1375.867</v>
+        <v>1379.105</v>
       </c>
       <c r="AB14" s="4">
         <f>AB46*AB5</f>
-        <v>1195.4820747527506</v>
+        <v>1182.6304747527504</v>
       </c>
       <c r="AC14" s="4">
         <f>AC46*AC5</f>
-        <v>1052.2010621291256</v>
+        <v>1047.3817121291254</v>
       </c>
       <c r="AD14" s="4">
         <f>AD46*AD5</f>
         <v>1207.7905681936882</v>
       </c>
       <c r="AE14" s="4">
-        <f t="shared" ref="AE14:AK14" si="17">AE46*AE5</f>
+        <f t="shared" ref="AE14:AK14" si="18">AE46*AE5</f>
         <v>1194.9074687996224</v>
       </c>
       <c r="AF14" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1254.6528422396034</v>
       </c>
       <c r="AG14" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1211.6361733628171</v>
       </c>
       <c r="AH14" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1260.1016202973299</v>
       </c>
       <c r="AI14" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1310.5056851092231</v>
       </c>
       <c r="AJ14" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1362.925912513592</v>
       </c>
       <c r="AK14" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1417.4429490141358</v>
       </c>
     </row>
@@ -2631,6 +2652,10 @@
       <c r="I15" s="4">
         <v>186.55</v>
       </c>
+      <c r="J15" s="4">
+        <f t="shared" si="17"/>
+        <v>202.10399999999996</v>
+      </c>
       <c r="S15" s="4">
         <v>273.14699999999999</v>
       </c>
@@ -2656,47 +2681,46 @@
         <v>700.84500000000003</v>
       </c>
       <c r="AA15" s="4">
-        <f>G15+H15+I15+I15</f>
-        <v>733.77600000000007</v>
+        <v>749.33</v>
       </c>
       <c r="AB15" s="4">
         <f>AB49*AB5</f>
-        <v>777.0633485892879</v>
+        <v>768.70980858928772</v>
       </c>
       <c r="AC15" s="4">
         <f>AC49*AC5</f>
-        <v>841.76084970330044</v>
+        <v>837.90536970330038</v>
       </c>
       <c r="AD15" s="4">
         <f>AD49*AD5</f>
         <v>885.71308334203798</v>
       </c>
       <c r="AE15" s="4">
-        <f t="shared" ref="AE15:AK15" si="18">AE49*AE5</f>
+        <f t="shared" ref="AE15:AK15" si="19">AE49*AE5</f>
         <v>853.50533485687311</v>
       </c>
       <c r="AF15" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>806.5625414397449</v>
       </c>
       <c r="AG15" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>838.82504309733474</v>
       </c>
       <c r="AH15" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>872.37804482122829</v>
       </c>
       <c r="AI15" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>806.46503699029108</v>
       </c>
       <c r="AJ15" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>838.72363846990277</v>
       </c>
       <c r="AK15" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>872.27258400869891</v>
       </c>
     </row>
@@ -2704,6 +2728,10 @@
       <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
+      <c r="J16" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="Y16" s="4">
         <v>1607.8</v>
       </c>
@@ -2713,59 +2741,59 @@
         <v>34</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" ref="C17:J17" si="19">+C13-C14-C15</f>
+        <f t="shared" ref="C17:J17" si="20">+C13-C14-C15</f>
         <v>-571.23</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-605.13499999999999</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-689.1</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-686.87800000000004</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-688.73200000000008</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-396.88849999999991</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-185.25000000000011</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <f t="shared" si="20"/>
+        <v>-280.87950000000001</v>
       </c>
       <c r="S17" s="5">
-        <f t="shared" ref="S17:X17" si="20">+S13-S14-S15</f>
+        <f t="shared" ref="S17:X17" si="21">+S13-S14-S15</f>
         <v>502.92100000000022</v>
       </c>
       <c r="T17" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>702.51000000000022</v>
       </c>
       <c r="U17" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>925.52900000000045</v>
       </c>
       <c r="V17" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1048.8200000000002</v>
       </c>
       <c r="W17" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1219.0399999999995</v>
       </c>
       <c r="X17" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1177.9899999999991</v>
       </c>
       <c r="Y17" s="5">
@@ -2778,46 +2806,46 @@
       </c>
       <c r="AA17" s="5">
         <f>+AA13-AA14-AA15</f>
-        <v>-1456.1204999999991</v>
+        <v>-1551.7500000000005</v>
       </c>
       <c r="AB17" s="5">
-        <f t="shared" ref="AB17:AK17" si="21">+AB13-AB14-AB15</f>
-        <v>-430.32501026004934</v>
+        <f t="shared" ref="AB17:AK17" si="22">+AB13-AB14-AB15</f>
+        <v>-465.52462026005048</v>
       </c>
       <c r="AC17" s="5">
-        <f t="shared" si="21"/>
-        <v>496.82959080213936</v>
+        <f t="shared" si="22"/>
+        <v>473.37542080213882</v>
       </c>
       <c r="AD17" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1164.4210049864923</v>
       </c>
       <c r="AE17" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1544.1532667213501</v>
       </c>
       <c r="AF17" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1799.9486797536697</v>
       </c>
       <c r="AG17" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2005.9392687323552</v>
       </c>
       <c r="AH17" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2128.2510299212709</v>
       </c>
       <c r="AI17" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2351.6154807899602</v>
       </c>
       <c r="AJ17" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2484.317764705861</v>
       </c>
       <c r="AK17" s="5">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2623.5789105855156</v>
       </c>
     </row>
@@ -2847,6 +2875,10 @@
       <c r="I18" s="4">
         <v>-152.33000000000001</v>
       </c>
+      <c r="J18" s="4">
+        <f t="shared" ref="J18:J19" si="23">+AA18-I18-H18-G18</f>
+        <v>-177.1049999999999</v>
+      </c>
       <c r="S18" s="4">
         <v>-151.75</v>
       </c>
@@ -2872,48 +2904,47 @@
         <v>-2072.9250000000002</v>
       </c>
       <c r="AA18" s="4">
-        <f>G18+H18+I18+I18</f>
-        <v>-776.73700000000008</v>
+        <v>-801.51199999999994</v>
       </c>
       <c r="AB18" s="4">
         <f>AA32*AB51</f>
-        <v>-911.12633500000015</v>
+        <v>-903.22981000000016</v>
       </c>
       <c r="AC18" s="4">
-        <f t="shared" ref="AC18:AK18" si="22">AB32*AC51</f>
-        <v>-1004.0889132265215</v>
+        <f t="shared" ref="AC18:AK18" si="24">AB32*AC51</f>
+        <v>-998.08449201702172</v>
       </c>
       <c r="AD18" s="4">
-        <f t="shared" si="22"/>
-        <v>-890.62666586372791</v>
+        <f t="shared" si="24"/>
+        <v>-886.51129926624662</v>
       </c>
       <c r="AE18" s="4">
-        <f t="shared" si="22"/>
-        <v>-728.77296560275784</v>
+        <f t="shared" si="24"/>
+        <v>-725.14184047491358</v>
       </c>
       <c r="AF18" s="4">
-        <f t="shared" si="22"/>
-        <v>-620.12085833090373</v>
+        <f t="shared" si="24"/>
+        <v>-616.69353010085979</v>
       </c>
       <c r="AG18" s="4">
-        <f t="shared" si="22"/>
-        <v>-568.62137392580007</v>
+        <f t="shared" si="24"/>
+        <v>-565.04444281851465</v>
       </c>
       <c r="AH18" s="4">
-        <f t="shared" si="22"/>
-        <v>-506.20584434382539</v>
+        <f t="shared" si="24"/>
+        <v>-502.47358500320615</v>
       </c>
       <c r="AI18" s="4">
-        <f t="shared" si="22"/>
-        <v>-436.13349232687972</v>
+        <f t="shared" si="24"/>
+        <v>-432.23999938274579</v>
       </c>
       <c r="AJ18" s="4">
-        <f t="shared" si="22"/>
-        <v>-353.38467042527463</v>
+        <f t="shared" si="24"/>
+        <v>-349.3229785859541</v>
       </c>
       <c r="AK18" s="4">
-        <f t="shared" si="22"/>
-        <v>-261.32836075235332</v>
+        <f t="shared" si="24"/>
+        <v>-257.09120382557415</v>
       </c>
     </row>
     <row r="19" spans="2:128" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2942,6 +2973,10 @@
       <c r="I19" s="4">
         <v>31.46</v>
       </c>
+      <c r="J19" s="4">
+        <f t="shared" si="23"/>
+        <v>-24.003999999999994</v>
+      </c>
       <c r="S19" s="4">
         <v>-10.85</v>
       </c>
@@ -2967,8 +3002,7 @@
         <v>123.953</v>
       </c>
       <c r="AA19" s="4">
-        <f>G19+H19+I19+I19</f>
-        <v>132.03</v>
+        <v>76.566000000000003</v>
       </c>
     </row>
     <row r="20" spans="2:128" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2976,112 +3010,112 @@
         <v>37</v>
       </c>
       <c r="C20" s="4">
-        <f t="shared" ref="C20:J20" si="23">+C17+C18+C19</f>
+        <f t="shared" ref="C20:J20" si="25">+C17+C18+C19</f>
         <v>-1368.4270000000001</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>-716.89400000000001</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>-845.57999999999993</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>-1570.414</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>-978.31200000000001</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>-510.27549999999997</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>-306.12000000000018</v>
       </c>
       <c r="J20" s="4">
-        <f t="shared" si="23"/>
-        <v>0</v>
+        <f t="shared" si="25"/>
+        <v>-481.98849999999993</v>
       </c>
       <c r="S20" s="4">
-        <f t="shared" ref="S20:AA20" si="24">+S17+S18+S19</f>
+        <f t="shared" ref="S20:AA20" si="26">+S17+S18+S19</f>
         <v>340.3210000000002</v>
       </c>
       <c r="T20" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>433.91000000000025</v>
       </c>
       <c r="U20" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>640.37900000000047</v>
       </c>
       <c r="V20" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>770.61600000000021</v>
       </c>
       <c r="W20" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>969.28999999999951</v>
       </c>
       <c r="X20" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>911.27799999999911</v>
       </c>
       <c r="Y20" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>-3999.99</v>
       </c>
       <c r="Z20" s="4">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>-4501.3149999999996</v>
       </c>
       <c r="AA20" s="4">
-        <f t="shared" si="24"/>
-        <v>-2100.827499999999</v>
+        <f t="shared" si="26"/>
+        <v>-2276.6960000000008</v>
       </c>
       <c r="AB20" s="4">
-        <f t="shared" ref="AB20:AK20" si="25">+AB17+AB18+AB19</f>
-        <v>-1341.4513452600495</v>
+        <f t="shared" ref="AB20:AK20" si="27">+AB17+AB18+AB19</f>
+        <v>-1368.7544302600506</v>
       </c>
       <c r="AC20" s="4">
-        <f t="shared" si="25"/>
-        <v>-507.25932242438216</v>
+        <f t="shared" si="27"/>
+        <v>-524.7090712148829</v>
       </c>
       <c r="AD20" s="4">
-        <f t="shared" si="25"/>
-        <v>273.79433912276443</v>
+        <f t="shared" si="27"/>
+        <v>277.90970572024571</v>
       </c>
       <c r="AE20" s="4">
-        <f t="shared" si="25"/>
-        <v>815.38030111859223</v>
+        <f t="shared" si="27"/>
+        <v>819.01142624643649</v>
       </c>
       <c r="AF20" s="4">
-        <f t="shared" si="25"/>
-        <v>1179.827821422766</v>
+        <f t="shared" si="27"/>
+        <v>1183.2551496528099</v>
       </c>
       <c r="AG20" s="4">
-        <f t="shared" si="25"/>
-        <v>1437.3178948065552</v>
+        <f t="shared" si="27"/>
+        <v>1440.8948259138406</v>
       </c>
       <c r="AH20" s="4">
-        <f t="shared" si="25"/>
-        <v>1622.0451855774454</v>
+        <f t="shared" si="27"/>
+        <v>1625.7774449180647</v>
       </c>
       <c r="AI20" s="4">
-        <f t="shared" si="25"/>
-        <v>1915.4819884630806</v>
+        <f t="shared" si="27"/>
+        <v>1919.3754814072145</v>
       </c>
       <c r="AJ20" s="4">
-        <f t="shared" si="25"/>
-        <v>2130.9330942805864</v>
+        <f t="shared" si="27"/>
+        <v>2134.9947861199071</v>
       </c>
       <c r="AK20" s="4">
-        <f t="shared" si="25"/>
-        <v>2362.250549833162</v>
+        <f t="shared" si="27"/>
+        <v>2366.4877067599414</v>
       </c>
     </row>
     <row r="21" spans="2:128" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3110,6 +3144,10 @@
       <c r="I21" s="4">
         <v>10.705</v>
       </c>
+      <c r="J21" s="4">
+        <f>+AA21-I21-H21-G21</f>
+        <v>-0.38200000000000056</v>
+      </c>
       <c r="S21" s="4">
         <v>2.2669999999999999</v>
       </c>
@@ -3135,48 +3173,47 @@
         <v>-5.2670000000000003</v>
       </c>
       <c r="AA21" s="4">
-        <f>G21+H21+I21+I21</f>
-        <v>17.887</v>
+        <v>6.8</v>
       </c>
       <c r="AB21" s="4">
         <f>AB20*-AB52</f>
-        <v>13.414513452600495</v>
+        <v>13.687544302600507</v>
       </c>
       <c r="AC21" s="4">
-        <f t="shared" ref="AC21:AK21" si="26">AC20*-AC52</f>
-        <v>7.6088898363657318</v>
+        <f t="shared" ref="AC21:AK21" si="28">AC20*-AC52</f>
+        <v>7.8706360682232432</v>
       </c>
       <c r="AD21" s="4">
-        <f t="shared" si="26"/>
-        <v>-5.475886782455289</v>
+        <f t="shared" si="28"/>
+        <v>-5.5581941144049143</v>
       </c>
       <c r="AE21" s="4">
-        <f t="shared" si="26"/>
-        <v>-20.384507527964807</v>
+        <f t="shared" si="28"/>
+        <v>-20.475285656160914</v>
       </c>
       <c r="AF21" s="4">
-        <f t="shared" si="26"/>
-        <v>-35.39483464268298</v>
+        <f t="shared" si="28"/>
+        <v>-35.497654489584299</v>
       </c>
       <c r="AG21" s="4">
-        <f t="shared" si="26"/>
-        <v>-50.306126318229438</v>
+        <f t="shared" si="28"/>
+        <v>-50.431318906984423</v>
       </c>
       <c r="AH21" s="4">
-        <f t="shared" si="26"/>
-        <v>-64.881807423097811</v>
+        <f t="shared" si="28"/>
+        <v>-65.031097796722591</v>
       </c>
       <c r="AI21" s="4">
-        <f t="shared" si="26"/>
-        <v>-76.61927953852323</v>
+        <f t="shared" si="28"/>
+        <v>-76.775019256288587</v>
       </c>
       <c r="AJ21" s="4">
-        <f t="shared" si="26"/>
-        <v>-85.237323771223458</v>
+        <f t="shared" si="28"/>
+        <v>-85.399791444796278</v>
       </c>
       <c r="AK21" s="4">
-        <f t="shared" si="26"/>
-        <v>-94.490021993326479</v>
+        <f t="shared" si="28"/>
+        <v>-94.659508270397652</v>
       </c>
     </row>
     <row r="22" spans="2:128" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -3184,476 +3221,476 @@
         <v>39</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" ref="C22:J22" si="27">+C20+C21</f>
+        <f t="shared" ref="C22:J22" si="29">+C20+C21</f>
         <v>-1370.1550000000002</v>
       </c>
       <c r="D22" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>-717.82100000000003</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>-845.87399999999991</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>-1572.732</v>
       </c>
       <c r="G22" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>-982.702</v>
       </c>
       <c r="H22" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>-509.40849999999995</v>
       </c>
       <c r="I22" s="5">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>-295.41500000000019</v>
       </c>
       <c r="J22" s="5">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f t="shared" si="29"/>
+        <v>-482.37049999999994</v>
       </c>
       <c r="S22" s="5">
-        <f t="shared" ref="S22:AA22" si="28">+S20+S21</f>
+        <f t="shared" ref="S22:AA22" si="30">+S20+S21</f>
         <v>342.58800000000019</v>
       </c>
       <c r="T22" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>427.14000000000027</v>
       </c>
       <c r="U22" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>633.17900000000043</v>
       </c>
       <c r="V22" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>759.87400000000025</v>
       </c>
       <c r="W22" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>954.78999999999951</v>
       </c>
       <c r="X22" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>930.13799999999912</v>
       </c>
       <c r="Y22" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>-4012.49</v>
       </c>
       <c r="Z22" s="5">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>-4506.5819999999994</v>
       </c>
       <c r="AA22" s="5">
-        <f t="shared" si="28"/>
-        <v>-2082.9404999999988</v>
+        <f t="shared" si="30"/>
+        <v>-2269.8960000000006</v>
       </c>
       <c r="AB22" s="5">
-        <f t="shared" ref="AB22:AK22" si="29">+AB20+AB21</f>
-        <v>-1328.0368318074491</v>
+        <f t="shared" ref="AB22:AK22" si="31">+AB20+AB21</f>
+        <v>-1355.06688595745</v>
       </c>
       <c r="AC22" s="5">
-        <f t="shared" si="29"/>
-        <v>-499.65043258801643</v>
+        <f t="shared" si="31"/>
+        <v>-516.83843514665966</v>
       </c>
       <c r="AD22" s="5">
-        <f t="shared" si="29"/>
-        <v>268.31845234030914</v>
+        <f t="shared" si="31"/>
+        <v>272.35151160584081</v>
       </c>
       <c r="AE22" s="5">
-        <f t="shared" si="29"/>
-        <v>794.99579359062739</v>
+        <f t="shared" si="31"/>
+        <v>798.53614059027552</v>
       </c>
       <c r="AF22" s="5">
-        <f t="shared" si="29"/>
-        <v>1144.432986780083</v>
+        <f t="shared" si="31"/>
+        <v>1147.7574951632257</v>
       </c>
       <c r="AG22" s="5">
-        <f t="shared" si="29"/>
-        <v>1387.0117684883257</v>
+        <f t="shared" si="31"/>
+        <v>1390.4635070068562</v>
       </c>
       <c r="AH22" s="5">
-        <f t="shared" si="29"/>
-        <v>1557.1633781543476</v>
+        <f t="shared" si="31"/>
+        <v>1560.7463471213421</v>
       </c>
       <c r="AI22" s="5">
-        <f t="shared" si="29"/>
-        <v>1838.8627089245574</v>
+        <f t="shared" si="31"/>
+        <v>1842.600462150926</v>
       </c>
       <c r="AJ22" s="5">
-        <f t="shared" si="29"/>
-        <v>2045.695770509363</v>
+        <f t="shared" si="31"/>
+        <v>2049.5949946751107</v>
       </c>
       <c r="AK22" s="5">
-        <f t="shared" si="29"/>
-        <v>2267.7605278398355</v>
+        <f t="shared" si="31"/>
+        <v>2271.8281984895439</v>
       </c>
       <c r="AL22" s="5">
         <f>AK22*(1+Dash!$C$2)</f>
-        <v>2245.082922561437</v>
+        <v>2249.1099165046485</v>
       </c>
       <c r="AM22" s="5">
         <f>AL22*(1+Dash!$C$2)</f>
-        <v>2222.6320933358224</v>
+        <v>2226.6188173396022</v>
       </c>
       <c r="AN22" s="5">
         <f>AM22*(1+Dash!$C$2)</f>
-        <v>2200.4057724024642</v>
+        <v>2204.352629166206</v>
       </c>
       <c r="AO22" s="5">
         <f>AN22*(1+Dash!$C$2)</f>
-        <v>2178.4017146784395</v>
+        <v>2182.3091028745439</v>
       </c>
       <c r="AP22" s="5">
         <f>AO22*(1+Dash!$C$2)</f>
-        <v>2156.6176975316553</v>
+        <v>2160.4860118457987</v>
       </c>
       <c r="AQ22" s="5">
         <f>AP22*(1+Dash!$C$2)</f>
-        <v>2135.0515205563388</v>
+        <v>2138.8811517273407</v>
       </c>
       <c r="AR22" s="5">
         <f>AQ22*(1+Dash!$C$2)</f>
-        <v>2113.7010053507752</v>
+        <v>2117.4923402100671</v>
       </c>
       <c r="AS22" s="5">
         <f>AR22*(1+Dash!$C$2)</f>
-        <v>2092.5639952972674</v>
+        <v>2096.3174168079663</v>
       </c>
       <c r="AT22" s="5">
         <f>AS22*(1+Dash!$C$2)</f>
-        <v>2071.6383553442947</v>
+        <v>2075.3542426398867</v>
       </c>
       <c r="AU22" s="5">
         <f>AT22*(1+Dash!$C$2)</f>
-        <v>2050.9219717908518</v>
+        <v>2054.6007002134879</v>
       </c>
       <c r="AV22" s="5">
         <f>AU22*(1+Dash!$C$2)</f>
-        <v>2030.4127520729432</v>
+        <v>2034.054693211353</v>
       </c>
       <c r="AW22" s="5">
         <f>AV22*(1+Dash!$C$2)</f>
-        <v>2010.1086245522138</v>
+        <v>2013.7141462792395</v>
       </c>
       <c r="AX22" s="5">
         <f>AW22*(1+Dash!$C$2)</f>
-        <v>1990.0075383066917</v>
+        <v>1993.577004816447</v>
       </c>
       <c r="AY22" s="5">
         <f>AX22*(1+Dash!$C$2)</f>
-        <v>1970.1074629236248</v>
+        <v>1973.6412347682826</v>
       </c>
       <c r="AZ22" s="5">
         <f>AY22*(1+Dash!$C$2)</f>
-        <v>1950.4063882943885</v>
+        <v>1953.9048224205999</v>
       </c>
       <c r="BA22" s="5">
         <f>AZ22*(1+Dash!$C$2)</f>
-        <v>1930.9023244114446</v>
+        <v>1934.3657741963939</v>
       </c>
       <c r="BB22" s="5">
         <f>BA22*(1+Dash!$C$2)</f>
-        <v>1911.5933011673301</v>
+        <v>1915.02211645443</v>
       </c>
       <c r="BC22" s="5">
         <f>BB22*(1+Dash!$C$2)</f>
-        <v>1892.4773681556567</v>
+        <v>1895.8718952898857</v>
       </c>
       <c r="BD22" s="5">
         <f>BC22*(1+Dash!$C$2)</f>
-        <v>1873.5525944741</v>
+        <v>1876.9131763369869</v>
       </c>
       <c r="BE22" s="5">
         <f>BD22*(1+Dash!$C$2)</f>
-        <v>1854.8170685293589</v>
+        <v>1858.1440445736171</v>
       </c>
       <c r="BF22" s="5">
         <f>BE22*(1+Dash!$C$2)</f>
-        <v>1836.2688978440654</v>
+        <v>1839.5626041278808</v>
       </c>
       <c r="BG22" s="5">
         <f>BF22*(1+Dash!$C$2)</f>
-        <v>1817.9062088656246</v>
+        <v>1821.1669780866021</v>
       </c>
       <c r="BH22" s="5">
         <f>BG22*(1+Dash!$C$2)</f>
-        <v>1799.7271467769683</v>
+        <v>1802.955308305736</v>
       </c>
       <c r="BI22" s="5">
         <f>BH22*(1+Dash!$C$2)</f>
-        <v>1781.7298753091986</v>
+        <v>1784.9257552226786</v>
       </c>
       <c r="BJ22" s="5">
         <f>BI22*(1+Dash!$C$2)</f>
-        <v>1763.9125765561066</v>
+        <v>1767.0764976704518</v>
       </c>
       <c r="BK22" s="5">
         <f>BJ22*(1+Dash!$C$2)</f>
-        <v>1746.2734507905454</v>
+        <v>1749.4057326937473</v>
       </c>
       <c r="BL22" s="5">
         <f>BK22*(1+Dash!$C$2)</f>
-        <v>1728.81071628264</v>
+        <v>1731.9116753668097</v>
       </c>
       <c r="BM22" s="5">
         <f>BL22*(1+Dash!$C$2)</f>
-        <v>1711.5226091198135</v>
+        <v>1714.5925586131416</v>
       </c>
       <c r="BN22" s="5">
         <f>BM22*(1+Dash!$C$2)</f>
-        <v>1694.4073830286154</v>
+        <v>1697.4466330270102</v>
       </c>
       <c r="BO22" s="5">
         <f>BN22*(1+Dash!$C$2)</f>
-        <v>1677.4633091983292</v>
+        <v>1680.47216669674</v>
       </c>
       <c r="BP22" s="5">
         <f>BO22*(1+Dash!$C$2)</f>
-        <v>1660.6886761063458</v>
+        <v>1663.6674450297726</v>
       </c>
       <c r="BQ22" s="5">
         <f>BP22*(1+Dash!$C$2)</f>
-        <v>1644.0817893452825</v>
+        <v>1647.0307705794748</v>
       </c>
       <c r="BR22" s="5">
         <f>BQ22*(1+Dash!$C$2)</f>
-        <v>1627.6409714518297</v>
+        <v>1630.5604628736801</v>
       </c>
       <c r="BS22" s="5">
         <f>BR22*(1+Dash!$C$2)</f>
-        <v>1611.3645617373113</v>
+        <v>1614.2548582449433</v>
       </c>
       <c r="BT22" s="5">
         <f>BS22*(1+Dash!$C$2)</f>
-        <v>1595.2509161199382</v>
+        <v>1598.1123096624938</v>
       </c>
       <c r="BU22" s="5">
         <f>BT22*(1+Dash!$C$2)</f>
-        <v>1579.2984069587387</v>
+        <v>1582.1311865658688</v>
       </c>
       <c r="BV22" s="5">
         <f>BU22*(1+Dash!$C$2)</f>
-        <v>1563.5054228891513</v>
+        <v>1566.30987470021</v>
       </c>
       <c r="BW22" s="5">
         <f>BV22*(1+Dash!$C$2)</f>
-        <v>1547.8703686602598</v>
+        <v>1550.6467759532079</v>
       </c>
       <c r="BX22" s="5">
         <f>BW22*(1+Dash!$C$2)</f>
-        <v>1532.3916649736573</v>
+        <v>1535.1403081936758</v>
       </c>
       <c r="BY22" s="5">
         <f>BX22*(1+Dash!$C$2)</f>
-        <v>1517.0677483239208</v>
+        <v>1519.788905111739</v>
       </c>
       <c r="BZ22" s="5">
         <f>BY22*(1+Dash!$C$2)</f>
-        <v>1501.8970708406816</v>
+        <v>1504.5910160606215</v>
       </c>
       <c r="CA22" s="5">
         <f>BZ22*(1+Dash!$C$2)</f>
-        <v>1486.8781001322748</v>
+        <v>1489.5451059000154</v>
       </c>
       <c r="CB22" s="5">
         <f>CA22*(1+Dash!$C$2)</f>
-        <v>1472.009319130952</v>
+        <v>1474.6496548410153</v>
       </c>
       <c r="CC22" s="5">
         <f>CB22*(1+Dash!$C$2)</f>
-        <v>1457.2892259396424</v>
+        <v>1459.903158292605</v>
       </c>
       <c r="CD22" s="5">
         <f>CC22*(1+Dash!$C$2)</f>
-        <v>1442.716333680246</v>
+        <v>1445.3041267096789</v>
       </c>
       <c r="CE22" s="5">
         <f>CD22*(1+Dash!$C$2)</f>
-        <v>1428.2891703434434</v>
+        <v>1430.8510854425822</v>
       </c>
       <c r="CF22" s="5">
         <f>CE22*(1+Dash!$C$2)</f>
-        <v>1414.006278640009</v>
+        <v>1416.5425745881564</v>
       </c>
       <c r="CG22" s="5">
         <f>CF22*(1+Dash!$C$2)</f>
-        <v>1399.866215853609</v>
+        <v>1402.3771488422749</v>
       </c>
       <c r="CH22" s="5">
         <f>CG22*(1+Dash!$C$2)</f>
-        <v>1385.867553695073</v>
+        <v>1388.3533773538522</v>
       </c>
       <c r="CI22" s="5">
         <f>CH22*(1+Dash!$C$2)</f>
-        <v>1372.0088781581221</v>
+        <v>1374.4698435803136</v>
       </c>
       <c r="CJ22" s="5">
         <f>CI22*(1+Dash!$C$2)</f>
-        <v>1358.288789376541</v>
+        <v>1360.7251451445104</v>
       </c>
       <c r="CK22" s="5">
         <f>CJ22*(1+Dash!$C$2)</f>
-        <v>1344.7059014827755</v>
+        <v>1347.1178936930653</v>
       </c>
       <c r="CL22" s="5">
         <f>CK22*(1+Dash!$C$2)</f>
-        <v>1331.2588424679477</v>
+        <v>1333.6467147561345</v>
       </c>
       <c r="CM22" s="5">
         <f>CL22*(1+Dash!$C$2)</f>
-        <v>1317.9462540432683</v>
+        <v>1320.3102476085733</v>
       </c>
       <c r="CN22" s="5">
         <f>CM22*(1+Dash!$C$2)</f>
-        <v>1304.7667915028355</v>
+        <v>1307.1071451324876</v>
       </c>
       <c r="CO22" s="5">
         <f>CN22*(1+Dash!$C$2)</f>
-        <v>1291.7191235878072</v>
+        <v>1294.0360736811626</v>
       </c>
       <c r="CP22" s="5">
         <f>CO22*(1+Dash!$C$2)</f>
-        <v>1278.8019323519291</v>
+        <v>1281.0957129443509</v>
       </c>
       <c r="CQ22" s="5">
         <f>CP22*(1+Dash!$C$2)</f>
-        <v>1266.0139130284097</v>
+        <v>1268.2847558149074</v>
       </c>
       <c r="CR22" s="5">
         <f>CQ22*(1+Dash!$C$2)</f>
-        <v>1253.3537738981256</v>
+        <v>1255.6019082567584</v>
       </c>
       <c r="CS22" s="5">
         <f>CR22*(1+Dash!$C$2)</f>
-        <v>1240.8202361591443</v>
+        <v>1243.0458891741907</v>
       </c>
       <c r="CT22" s="5">
         <f>CS22*(1+Dash!$C$2)</f>
-        <v>1228.4120337975528</v>
+        <v>1230.6154302824489</v>
       </c>
       <c r="CU22" s="5">
         <f>CT22*(1+Dash!$C$2)</f>
-        <v>1216.1279134595773</v>
+        <v>1218.3092759796243</v>
       </c>
       <c r="CV22" s="5">
         <f>CU22*(1+Dash!$C$2)</f>
-        <v>1203.9666343249814</v>
+        <v>1206.1261832198281</v>
       </c>
       <c r="CW22" s="5">
         <f>CV22*(1+Dash!$C$2)</f>
-        <v>1191.9269679817317</v>
+        <v>1194.0649213876297</v>
       </c>
       <c r="CX22" s="5">
         <f>CW22*(1+Dash!$C$2)</f>
-        <v>1180.0076983019144</v>
+        <v>1182.1242721737535</v>
       </c>
       <c r="CY22" s="5">
         <f>CX22*(1+Dash!$C$2)</f>
-        <v>1168.2076213188952</v>
+        <v>1170.3030294520161</v>
       </c>
       <c r="CZ22" s="5">
         <f>CY22*(1+Dash!$C$2)</f>
-        <v>1156.5255451057062</v>
+        <v>1158.5999991574959</v>
       </c>
       <c r="DA22" s="5">
         <f>CZ22*(1+Dash!$C$2)</f>
-        <v>1144.9602896546492</v>
+        <v>1147.0139991659209</v>
       </c>
       <c r="DB22" s="5">
         <f>DA22*(1+Dash!$C$2)</f>
-        <v>1133.5106867581026</v>
+        <v>1135.5438591742618</v>
       </c>
       <c r="DC22" s="5">
         <f>DB22*(1+Dash!$C$2)</f>
-        <v>1122.1755798905215</v>
+        <v>1124.1884205825193</v>
       </c>
       <c r="DD22" s="5">
         <f>DC22*(1+Dash!$C$2)</f>
-        <v>1110.9538240916163</v>
+        <v>1112.946536376694</v>
       </c>
       <c r="DE22" s="5">
         <f>DD22*(1+Dash!$C$2)</f>
-        <v>1099.8442858507001</v>
+        <v>1101.817071012927</v>
       </c>
       <c r="DF22" s="5">
         <f>DE22*(1+Dash!$C$2)</f>
-        <v>1088.8458429921932</v>
+        <v>1090.7989003027978</v>
       </c>
       <c r="DG22" s="5">
         <f>DF22*(1+Dash!$C$2)</f>
-        <v>1077.9573845622713</v>
+        <v>1079.8909112997699</v>
       </c>
       <c r="DH22" s="5">
         <f>DG22*(1+Dash!$C$2)</f>
-        <v>1067.1778107166485</v>
+        <v>1069.0920021867721</v>
       </c>
       <c r="DI22" s="5">
         <f>DH22*(1+Dash!$C$2)</f>
-        <v>1056.506032609482</v>
+        <v>1058.4010821649044</v>
       </c>
       <c r="DJ22" s="5">
         <f>DI22*(1+Dash!$C$2)</f>
-        <v>1045.9409722833871</v>
+        <v>1047.8170713432553</v>
       </c>
       <c r="DK22" s="5">
         <f>DJ22*(1+Dash!$C$2)</f>
-        <v>1035.4815625605531</v>
+        <v>1037.3389006298228</v>
       </c>
       <c r="DL22" s="5">
         <f>DK22*(1+Dash!$C$2)</f>
-        <v>1025.1267469349475</v>
+        <v>1026.9655116235244</v>
       </c>
       <c r="DM22" s="5">
         <f>DL22*(1+Dash!$C$2)</f>
-        <v>1014.875479465598</v>
+        <v>1016.6958565072891</v>
       </c>
       <c r="DN22" s="5">
         <f>DM22*(1+Dash!$C$2)</f>
-        <v>1004.726724670942</v>
+        <v>1006.5288979422162</v>
       </c>
       <c r="DO22" s="5">
         <f>DN22*(1+Dash!$C$2)</f>
-        <v>994.67945742423251</v>
+        <v>996.46360896279407</v>
       </c>
       <c r="DP22" s="5">
         <f>DO22*(1+Dash!$C$2)</f>
-        <v>984.73266284999022</v>
+        <v>986.49897287316617</v>
       </c>
       <c r="DQ22" s="5">
         <f>DP22*(1+Dash!$C$2)</f>
-        <v>974.88533622149032</v>
+        <v>976.63398314443452</v>
       </c>
       <c r="DR22" s="5">
         <f>DQ22*(1+Dash!$C$2)</f>
-        <v>965.13648285927536</v>
+        <v>966.86764331299014</v>
       </c>
       <c r="DS22" s="5">
         <f>DR22*(1+Dash!$C$2)</f>
-        <v>955.48511803068254</v>
+        <v>957.19896687986022</v>
       </c>
       <c r="DT22" s="5">
         <f>DS22*(1+Dash!$C$2)</f>
-        <v>945.93026685037569</v>
+        <v>947.62697721106156</v>
       </c>
       <c r="DU22" s="5">
         <f>DT22*(1+Dash!$C$2)</f>
-        <v>936.47096418187198</v>
+        <v>938.15070743895092</v>
       </c>
       <c r="DV22" s="5">
         <f>DU22*(1+Dash!$C$2)</f>
-        <v>927.10625454005321</v>
+        <v>928.76920036456136</v>
       </c>
       <c r="DW22" s="5">
         <f>DV22*(1+Dash!$C$2)</f>
-        <v>917.83519199465263</v>
+        <v>919.48150836091577</v>
       </c>
       <c r="DX22" s="5">
         <f>DW22*(1+Dash!$C$2)</f>
-        <v>908.65684007470611</v>
+        <v>910.28669327730665</v>
       </c>
     </row>
     <row r="23" spans="2:128" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -3681,6 +3718,9 @@
       <c r="I23" s="4">
         <v>420.79849999999999</v>
       </c>
+      <c r="J23" s="4">
+        <v>419.77300000000002</v>
+      </c>
       <c r="S23" s="4">
         <v>206.5249</v>
       </c>
@@ -3706,7 +3746,7 @@
         <v>365.44900000000001</v>
       </c>
       <c r="AA23" s="4">
-        <v>365.44900000000001</v>
+        <v>419.77300000000002</v>
       </c>
       <c r="AB23" s="4">
         <v>365.44900000000001</v>
@@ -3744,112 +3784,112 @@
         <v>40</v>
       </c>
       <c r="C24" s="6">
-        <f t="shared" ref="C24:J24" si="30">+C22/C23</f>
+        <f t="shared" ref="C24:J24" si="32">+C22/C23</f>
         <v>-4.1598381186300202</v>
       </c>
       <c r="D24" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-1.9404081279583061</v>
       </c>
       <c r="E24" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-2.2860446185628529</v>
       </c>
       <c r="F24" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-4.3035608251767004</v>
       </c>
       <c r="G24" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-2.3524559259529676</v>
       </c>
       <c r="H24" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-1.2154616840090953</v>
       </c>
       <c r="I24" s="6">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>-0.70203434660532349</v>
       </c>
-      <c r="J24" s="6" t="e">
-        <f t="shared" si="30"/>
-        <v>#DIV/0!</v>
+      <c r="J24" s="6">
+        <f t="shared" si="32"/>
+        <v>-1.1491222636996661</v>
       </c>
       <c r="S24" s="6">
-        <f t="shared" ref="S24:AA24" si="31">+S22/S23</f>
+        <f t="shared" ref="S24:AA24" si="33">+S22/S23</f>
         <v>1.6588217691910283</v>
       </c>
       <c r="T24" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1.8850704573438497</v>
       </c>
       <c r="U24" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>2.78784876783741</v>
       </c>
       <c r="V24" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>3.3321961059463265</v>
       </c>
       <c r="W24" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>4.2815311073443265</v>
       </c>
       <c r="X24" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>4.3276342658699374</v>
       </c>
       <c r="Y24" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>-15.75193341969929</v>
       </c>
       <c r="Z24" s="6">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>-12.331630405336995</v>
       </c>
       <c r="AA24" s="6">
-        <f t="shared" si="31"/>
-        <v>-5.6996749204403319</v>
+        <f t="shared" si="33"/>
+        <v>-5.4074368765975906</v>
       </c>
       <c r="AB24" s="6">
-        <f t="shared" ref="AB24:AK24" si="32">+AB22/AB23</f>
-        <v>-3.6339867719092105</v>
+        <f t="shared" ref="AB24:AK24" si="34">+AB22/AB23</f>
+        <v>-3.7079507289866713</v>
       </c>
       <c r="AC24" s="6">
-        <f t="shared" si="32"/>
-        <v>-1.3672234226609361</v>
+        <f t="shared" si="34"/>
+        <v>-1.4142559841363902</v>
       </c>
       <c r="AD24" s="6">
-        <f t="shared" si="32"/>
-        <v>0.73421586142063355</v>
+        <f t="shared" si="34"/>
+        <v>0.74525176318950337</v>
       </c>
       <c r="AE24" s="6">
-        <f t="shared" si="32"/>
-        <v>2.1753946339725307</v>
+        <f t="shared" si="34"/>
+        <v>2.1850822976400961</v>
       </c>
       <c r="AF24" s="6">
-        <f t="shared" si="32"/>
-        <v>3.131580567411822</v>
+        <f t="shared" si="34"/>
+        <v>3.14067761893787</v>
       </c>
       <c r="AG24" s="6">
-        <f t="shared" si="32"/>
-        <v>3.7953634255075968</v>
+        <f t="shared" si="34"/>
+        <v>3.8048086244779875</v>
       </c>
       <c r="AH24" s="6">
-        <f t="shared" si="32"/>
-        <v>4.2609594721954291</v>
+        <f t="shared" si="34"/>
+        <v>4.2707637649065724</v>
       </c>
       <c r="AI24" s="6">
-        <f t="shared" si="32"/>
-        <v>5.0317902331777002</v>
+        <f t="shared" si="34"/>
+        <v>5.0420180713339642</v>
       </c>
       <c r="AJ24" s="6">
-        <f t="shared" si="32"/>
-        <v>5.5977599350644356</v>
+        <f t="shared" si="34"/>
+        <v>5.6084296158290501</v>
       </c>
       <c r="AK24" s="6">
-        <f t="shared" si="32"/>
-        <v>6.2054090388531247</v>
+        <f t="shared" si="34"/>
+        <v>6.2165396498267711</v>
       </c>
     </row>
     <row r="25" spans="2:128" x14ac:dyDescent="0.25">
@@ -3857,140 +3897,148 @@
     </row>
     <row r="26" spans="2:128" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="4">
         <f>C17+C15</f>
         <v>-400.93</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" ref="D26:I26" si="33">D17+D15</f>
+        <f t="shared" ref="D26:I26" si="35">D17+D15</f>
         <v>-430.83499999999998</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>-515.81100000000004</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>-503.92200000000003</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>-509.65600000000006</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>-215.28849999999991</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" si="33"/>
+        <f t="shared" si="35"/>
         <v>1.2999999999998977</v>
       </c>
       <c r="J26" s="4">
         <f>J17+J15</f>
-        <v>0</v>
+        <v>-78.775500000000051</v>
       </c>
       <c r="S26" s="4">
-        <f t="shared" ref="S26:Z26" si="34">S17+S15</f>
+        <f t="shared" ref="S26:Z26" si="36">S17+S15</f>
         <v>776.06800000000021</v>
       </c>
       <c r="T26" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1134.6240000000003</v>
       </c>
       <c r="U26" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1358.0290000000005</v>
       </c>
       <c r="V26" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1558.777</v>
       </c>
       <c r="W26" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1780.0999999999995</v>
       </c>
       <c r="X26" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>1824.1899999999991</v>
       </c>
       <c r="Y26" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>-2766.29</v>
       </c>
       <c r="Z26" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
         <v>-1851.4979999999998</v>
+      </c>
+      <c r="AA26" s="4">
+        <f t="shared" ref="AA26" si="37">AA17+AA15</f>
+        <v>-802.42000000000041</v>
       </c>
     </row>
     <row r="27" spans="2:128" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="4">
         <f>+C22-C21-C18</f>
         <v>-543.98700000000008</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" ref="D27:J27" si="35">+D22-D21-D18</f>
+        <f t="shared" ref="D27:J27" si="38">+D22-D21-D18</f>
         <v>-579.63499999999999</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>-684.37999999999988</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>-620.38799999999992</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>-650.61200000000008</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>-365.89849999999996</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>-153.79000000000016</v>
       </c>
       <c r="J27" s="4">
-        <f t="shared" si="35"/>
-        <v>0</v>
+        <f t="shared" si="38"/>
+        <v>-304.88350000000003</v>
       </c>
       <c r="S27" s="4">
-        <f t="shared" ref="S27:Z27" si="36">+S22-S21-S18</f>
+        <f t="shared" ref="S27:Z27" si="39">+S22-S21-S18</f>
         <v>492.0710000000002</v>
       </c>
       <c r="T27" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>655.81000000000029</v>
       </c>
       <c r="U27" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>917.2290000000005</v>
       </c>
       <c r="V27" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1038.42</v>
       </c>
       <c r="W27" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1239.6899999999996</v>
       </c>
       <c r="X27" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1184.1449999999991</v>
       </c>
       <c r="Y27" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>-3517.6899999999996</v>
       </c>
       <c r="Z27" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>-2428.3899999999994</v>
+      </c>
+      <c r="AA27" s="4">
+        <f t="shared" ref="AA27" si="40">+AA22-AA21-AA18</f>
+        <v>-1475.1840000000009</v>
       </c>
     </row>
     <row r="28" spans="2:128" x14ac:dyDescent="0.25">
@@ -4003,6 +4051,10 @@
       <c r="I29" s="4">
         <v>1186.7</v>
       </c>
+      <c r="J29" s="4">
+        <f>946.987+0</f>
+        <v>946.98699999999997</v>
+      </c>
       <c r="S29" s="4">
         <v>84.823999999999998</v>
       </c>
@@ -4028,6 +4080,10 @@
         <f>1506.65+240</f>
         <v>1746.65</v>
       </c>
+      <c r="AA29" s="4">
+        <f>946.987+0</f>
+        <v>946.98699999999997</v>
+      </c>
     </row>
     <row r="30" spans="2:128" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
@@ -4037,6 +4093,10 @@
         <f>1012.7+141.3+12893.407</f>
         <v>14047.406999999999</v>
       </c>
+      <c r="J30" s="4">
+        <f>991.13+228.74+12630.4</f>
+        <v>13850.27</v>
+      </c>
       <c r="S30" s="4">
         <f>576.947+101.98+5503.076</f>
         <v>6182.0029999999997</v>
@@ -4069,6 +4129,10 @@
         <f>876.9+233.2+11569.7</f>
         <v>12679.800000000001</v>
       </c>
+      <c r="AA30" s="4">
+        <f>991.13+228.74+12630.4</f>
+        <v>13850.27</v>
+      </c>
     </row>
     <row r="31" spans="2:128" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
@@ -4077,6 +4141,9 @@
       <c r="I31" s="4">
         <v>14511.648999999999</v>
       </c>
+      <c r="J31" s="4">
+        <v>14516.366</v>
+      </c>
       <c r="S31" s="4">
         <v>8623.77</v>
       </c>
@@ -4100,6 +4167,9 @@
       </c>
       <c r="Z31" s="4">
         <v>13528.8</v>
+      </c>
+      <c r="AA31" s="4">
+        <v>14516.366</v>
       </c>
     </row>
     <row r="32" spans="2:128" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -4110,81 +4180,85 @@
         <f>+I29-I30</f>
         <v>-12860.706999999999</v>
       </c>
+      <c r="J32" s="5">
+        <f>+J29-J30</f>
+        <v>-12903.283000000001</v>
+      </c>
       <c r="S32" s="5">
-        <f t="shared" ref="S32:Z32" si="37">+S29-S30</f>
+        <f t="shared" ref="S32:AA32" si="41">+S29-S30</f>
         <v>-6097.1790000000001</v>
       </c>
       <c r="T32" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-6333.0029999999997</v>
       </c>
       <c r="U32" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-6308.3460000000005</v>
       </c>
       <c r="V32" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-6185.0429999999997</v>
       </c>
       <c r="W32" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-6487.8670000000002</v>
       </c>
       <c r="X32" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-6649.5940000000001</v>
       </c>
       <c r="Y32" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-8588.7210000000014</v>
       </c>
       <c r="Z32" s="5">
-        <f t="shared" si="37"/>
+        <f t="shared" si="41"/>
         <v>-10933.150000000001</v>
       </c>
       <c r="AA32" s="5">
-        <f>Z32+AA22</f>
-        <v>-13016.0905</v>
+        <f t="shared" si="41"/>
+        <v>-12903.283000000001</v>
       </c>
       <c r="AB32" s="5">
-        <f t="shared" ref="AB32:AK32" si="38">AA32+AB22</f>
-        <v>-14344.127331807449</v>
+        <f t="shared" ref="AB32:AK32" si="42">AA32+AB22</f>
+        <v>-14258.349885957452</v>
       </c>
       <c r="AC32" s="5">
-        <f t="shared" si="38"/>
-        <v>-14843.777764395465</v>
+        <f t="shared" si="42"/>
+        <v>-14775.188321104111</v>
       </c>
       <c r="AD32" s="5">
-        <f t="shared" si="38"/>
-        <v>-14575.459312055156</v>
+        <f t="shared" si="42"/>
+        <v>-14502.836809498271</v>
       </c>
       <c r="AE32" s="5">
-        <f t="shared" si="38"/>
-        <v>-13780.463518464529</v>
+        <f t="shared" si="42"/>
+        <v>-13704.300668907996</v>
       </c>
       <c r="AF32" s="5">
-        <f t="shared" si="38"/>
-        <v>-12636.030531684446</v>
+        <f t="shared" si="42"/>
+        <v>-12556.543173744771</v>
       </c>
       <c r="AG32" s="5">
-        <f t="shared" si="38"/>
-        <v>-11249.01876319612</v>
+        <f t="shared" si="42"/>
+        <v>-11166.079666737915</v>
       </c>
       <c r="AH32" s="5">
-        <f t="shared" si="38"/>
-        <v>-9691.855385041772</v>
+        <f t="shared" si="42"/>
+        <v>-9605.3333196165731</v>
       </c>
       <c r="AI32" s="5">
-        <f t="shared" si="38"/>
-        <v>-7852.9926761172146</v>
+        <f t="shared" si="42"/>
+        <v>-7762.7328574656476</v>
       </c>
       <c r="AJ32" s="5">
-        <f t="shared" si="38"/>
-        <v>-5807.2969056078518</v>
+        <f t="shared" si="42"/>
+        <v>-5713.1378627905369</v>
       </c>
       <c r="AK32" s="5">
-        <f t="shared" si="38"/>
-        <v>-3539.5363777680163</v>
+        <f t="shared" si="42"/>
+        <v>-3441.3096643009931</v>
       </c>
     </row>
     <row r="34" spans="2:37" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -4215,6 +4289,9 @@
       <c r="Z34" s="4">
         <v>2113.06</v>
       </c>
+      <c r="AA34" s="4">
+        <v>1770.17</v>
+      </c>
     </row>
     <row r="37" spans="2:37" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
@@ -4225,40 +4302,40 @@
         <v>0.39003192700935418</v>
       </c>
       <c r="U37" s="8">
-        <f t="shared" ref="U37:AB37" si="39">U5/T5-1</f>
+        <f t="shared" ref="U37:AB37" si="43">U5/T5-1</f>
         <v>0.12181176242608571</v>
       </c>
       <c r="V37" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>0.10705439120753235</v>
       </c>
       <c r="W37" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>0.12211242222500185</v>
       </c>
       <c r="X37" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>6.7259663937018432E-2</v>
       </c>
       <c r="Y37" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-0.80194448484923508</v>
       </c>
       <c r="Z37" s="8">
-        <f t="shared" si="39"/>
+        <f t="shared" si="43"/>
         <v>-0.4937284652827153</v>
       </c>
       <c r="AA37" s="8">
-        <f t="shared" si="39"/>
-        <v>6.6238954168480007</v>
+        <f t="shared" si="43"/>
+        <v>6.4751459145470101</v>
       </c>
       <c r="AB37" s="8">
-        <f t="shared" si="39"/>
-        <v>0.20996609488821916</v>
+        <f t="shared" si="43"/>
+        <v>0.22077732459158828</v>
       </c>
       <c r="AC37" s="8">
         <f>AC5/AB5-1</f>
-        <v>0.17353056071179962</v>
+        <v>0.18084979147646729</v>
       </c>
       <c r="AD37" s="8">
         <v>0.06</v>
@@ -4294,107 +4371,107 @@
         <v>-63.78387096774194</v>
       </c>
       <c r="D39" s="7">
-        <f t="shared" ref="D39:J39" si="40">D13/D5</f>
+        <f t="shared" ref="D39:J39" si="44">D13/D5</f>
         <v>-55.965328467153284</v>
       </c>
       <c r="E39" s="7">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-1.8726752503576543</v>
       </c>
       <c r="F39" s="7">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-0.4724804428241115</v>
       </c>
       <c r="G39" s="7">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>-0.4089413838357715</v>
       </c>
       <c r="H39" s="7">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>9.5849281329389052E-2</v>
       </c>
       <c r="I39" s="7">
-        <f t="shared" si="40"/>
+        <f t="shared" si="44"/>
         <v>0.23311049210770654</v>
       </c>
-      <c r="J39" s="7" t="e">
-        <f t="shared" si="40"/>
-        <v>#DIV/0!</v>
+      <c r="J39" s="7">
+        <f t="shared" si="44"/>
+        <v>0.1973207391418545</v>
       </c>
       <c r="S39" s="7">
-        <f t="shared" ref="S39:AK39" si="41">S13/S5</f>
+        <f t="shared" ref="S39:AK39" si="45">S13/S5</f>
         <v>0.37724992642072003</v>
       </c>
       <c r="T39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.38885974988222294</v>
       </c>
       <c r="U39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.41527246482303098</v>
       </c>
       <c r="V39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.43225655209477087</v>
       </c>
       <c r="W39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.4422754976577653</v>
       </c>
       <c r="X39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.43312835209319156</v>
       </c>
       <c r="Y39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-0.3228273863005991</v>
       </c>
       <c r="Z39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>-1.4815967110197505</v>
       </c>
       <c r="AA39" s="7">
-        <f t="shared" si="41"/>
-        <v>0.13228806754131017</v>
+        <f t="shared" ref="AA39" si="46">AA13/AA5</f>
+        <v>0.11905730259137519</v>
       </c>
       <c r="AB39" s="7">
-        <f t="shared" si="41"/>
-        <v>0.25800812001316725</v>
+        <f t="shared" si="45"/>
+        <v>0.25127302142161073</v>
       </c>
       <c r="AC39" s="7">
         <f>AC13/AC5</f>
-        <v>0.34082718436866138</v>
+        <v>0.33779411202051507</v>
       </c>
       <c r="AD39" s="7">
         <f>AD13/AD5</f>
         <v>0.40461377274140448</v>
       </c>
       <c r="AE39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.42091899413614026</v>
       </c>
       <c r="AF39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.43084664592613281</v>
       </c>
       <c r="AG39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.43522310960017835</v>
       </c>
       <c r="AH39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.43956374742576898</v>
       </c>
       <c r="AI39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.44327637260666725</v>
       </c>
       <c r="AJ39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.44696175004563293</v>
       </c>
       <c r="AK39" s="7">
-        <f t="shared" si="41"/>
+        <f t="shared" si="45"/>
         <v>0.45062009593637314</v>
       </c>
     </row>
@@ -4407,107 +4484,107 @@
         <v>-184.26774193548388</v>
       </c>
       <c r="D40" s="7">
-        <f t="shared" ref="D40:J40" si="42">D17/D5</f>
+        <f t="shared" ref="D40:J40" si="47">D17/D5</f>
         <v>-138.03261861313868</v>
       </c>
       <c r="E40" s="7">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>-4.5015384012385606</v>
       </c>
       <c r="F40" s="7">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>-1.4092204416341654</v>
       </c>
       <c r="G40" s="7">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>-1.3195237137301112</v>
       </c>
       <c r="H40" s="7">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>-0.33430860383156213</v>
       </c>
       <c r="I40" s="7">
-        <f t="shared" si="42"/>
+        <f t="shared" si="47"/>
         <v>-0.11467038068709384</v>
       </c>
-      <c r="J40" s="7" t="e">
-        <f t="shared" si="42"/>
-        <v>#DIV/0!</v>
+      <c r="J40" s="7">
+        <f t="shared" si="47"/>
+        <v>-0.18489704189220943</v>
       </c>
       <c r="S40" s="7">
-        <f t="shared" ref="S40:AK40" si="43">S17/S5</f>
+        <f t="shared" ref="S40:AK40" si="48">S17/S5</f>
         <v>0.16088941354114689</v>
       </c>
       <c r="T40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.16167967718839249</v>
       </c>
       <c r="U40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.18987726373587155</v>
       </c>
       <c r="V40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.19436360014269369</v>
       </c>
       <c r="W40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.20132400458125066</v>
       </c>
       <c r="X40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.18228423583880848</v>
       </c>
       <c r="Y40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>-2.7221367127376142</v>
       </c>
       <c r="Z40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>-3.9389103401020398</v>
       </c>
       <c r="AA40" s="7">
-        <f t="shared" si="43"/>
-        <v>-0.29475246384368703</v>
+        <f t="shared" ref="AA40" si="49">AA17/AA5</f>
+        <v>-0.32036062893289519</v>
       </c>
       <c r="AB40" s="7">
-        <f t="shared" si="43"/>
-        <v>-7.1991879986832777E-2</v>
+        <f t="shared" si="48"/>
+        <v>-7.8726978578389256E-2</v>
       </c>
       <c r="AC40" s="7">
         <f>AC17/AC5</f>
-        <v>7.0827184368661381E-2</v>
+        <v>6.7794112020515093E-2</v>
       </c>
       <c r="AD40" s="7">
         <f>AD17/AD5</f>
         <v>0.14461377274140449</v>
       </c>
       <c r="AE40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.18091899413614021</v>
       </c>
       <c r="AF40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.2008466459261328</v>
       </c>
       <c r="AG40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.21522310960017829</v>
       </c>
       <c r="AH40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.21956374742576901</v>
       </c>
       <c r="AI40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.23327637260666723</v>
       </c>
       <c r="AJ40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.23696175004563291</v>
       </c>
       <c r="AK40" s="7">
-        <f t="shared" si="43"/>
+        <f t="shared" si="48"/>
         <v>0.24062009593637315</v>
       </c>
     </row>
@@ -4520,107 +4597,107 @@
         <v>26.496129032258064</v>
       </c>
       <c r="D42" s="7">
-        <f t="shared" ref="D42:J42" si="44">D8/D$5</f>
+        <f t="shared" ref="D42:J42" si="50">D8/D$5</f>
         <v>19.765054744525546</v>
       </c>
       <c r="E42" s="7">
-        <f t="shared" si="44"/>
+        <f t="shared" si="50"/>
         <v>1.0088776530072314</v>
       </c>
       <c r="F42" s="7">
-        <f t="shared" si="44"/>
+        <f t="shared" si="50"/>
         <v>0.43948405574692717</v>
       </c>
       <c r="G42" s="7">
-        <f t="shared" si="44"/>
+        <f t="shared" si="50"/>
         <v>0.46120259409336062</v>
       </c>
       <c r="H42" s="7">
-        <f t="shared" si="44"/>
+        <f t="shared" si="50"/>
         <v>0.22119421289900876</v>
       </c>
       <c r="I42" s="7">
-        <f t="shared" si="44"/>
+        <f t="shared" si="50"/>
         <v>0.17790157845868151</v>
       </c>
-      <c r="J42" s="7" t="e">
-        <f t="shared" si="44"/>
-        <v>#DIV/0!</v>
+      <c r="J42" s="7">
+        <f t="shared" si="50"/>
+        <v>0.19610983514722083</v>
       </c>
       <c r="S42" s="7">
-        <f t="shared" ref="S42:AK42" si="45">S8/S$5</f>
+        <f t="shared" ref="S42:AK42" si="51">S8/S$5</f>
         <v>0.14480722228620418</v>
       </c>
       <c r="T42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.15330237259535109</v>
       </c>
       <c r="U42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.15307464332709522</v>
       </c>
       <c r="V42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.14892585952086432</v>
       </c>
       <c r="W42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.14559690443534104</v>
       </c>
       <c r="X42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.1430123267279238</v>
       </c>
       <c r="Y42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.40729426287785853</v>
       </c>
       <c r="Z42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.82940575509813552</v>
       </c>
       <c r="AA42" s="7">
-        <f t="shared" si="45"/>
-        <v>0.21823783786190973</v>
+        <f t="shared" ref="AA42" si="52">AA8/AA$5</f>
+        <v>0.22475101986886223</v>
       </c>
       <c r="AB42" s="7">
-        <f t="shared" si="45"/>
-        <v>0.19204373073007097</v>
+        <f t="shared" si="51"/>
+        <v>0.1950196131252768</v>
       </c>
       <c r="AC42" s="7">
-        <f t="shared" ref="AC42:AD44" si="46">AC8/AC$5</f>
-        <v>0.17359629547898137</v>
+        <f t="shared" ref="AC42:AD44" si="53">AC8/AC$5</f>
+        <v>0.17439506950465722</v>
       </c>
       <c r="AD42" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="53"/>
         <v>0.1592487112364239</v>
       </c>
       <c r="AE42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.1547416722391666</v>
       </c>
       <c r="AF42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.15179421181556343</v>
       </c>
       <c r="AG42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.15033465208656763</v>
       </c>
       <c r="AH42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.14888912658573525</v>
       </c>
       <c r="AI42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.1474575003685647</v>
       </c>
       <c r="AJ42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.14603963978809772</v>
       </c>
       <c r="AK42" s="7">
-        <f t="shared" si="45"/>
+        <f t="shared" si="51"/>
         <v>0.14463541248244294</v>
       </c>
     </row>
@@ -4629,111 +4706,111 @@
         <v>52</v>
       </c>
       <c r="C43" s="7">
-        <f t="shared" ref="C43:J43" si="47">C9/C$5</f>
+        <f t="shared" ref="C43:J43" si="54">C9/C$5</f>
         <v>13.741935483870968</v>
       </c>
       <c r="D43" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="54"/>
         <v>12.340328467153284</v>
       </c>
       <c r="E43" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="54"/>
         <v>0.51762138998308094</v>
       </c>
       <c r="F43" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="54"/>
         <v>0.25832500712941903</v>
       </c>
       <c r="G43" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="54"/>
         <v>0.25960092345125541</v>
       </c>
       <c r="H43" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="54"/>
         <v>0.15262906084272804</v>
       </c>
       <c r="I43" s="7">
-        <f t="shared" si="47"/>
+        <f t="shared" si="54"/>
         <v>0.11574373259052925</v>
       </c>
-      <c r="J43" s="7" t="e">
-        <f t="shared" si="47"/>
-        <v>#DIV/0!</v>
+      <c r="J43" s="7">
+        <f t="shared" si="54"/>
+        <v>0.12055785185170556</v>
       </c>
       <c r="S43" s="7">
-        <f t="shared" ref="S43:AK43" si="48">S9/S$5</f>
+        <f t="shared" ref="S43:AK43" si="55">S9/S$5</f>
         <v>0.10436421103817166</v>
       </c>
       <c r="T43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>8.2541766271820971E-2</v>
       </c>
       <c r="U43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>6.8761932350420177E-2</v>
       </c>
       <c r="V43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>6.6905168939109638E-2</v>
       </c>
       <c r="W43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>6.485425958053645E-2</v>
       </c>
       <c r="X43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>6.3382221410687709E-2</v>
       </c>
       <c r="Y43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>0.20681141642771755</v>
       </c>
       <c r="Z43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>0.46583084098015076</v>
       </c>
       <c r="AA43" s="7">
-        <f t="shared" si="48"/>
-        <v>0.13980717577837257</v>
+        <f t="shared" ref="AA43" si="56">AA9/AA$5</f>
+        <v>0.141795836292467</v>
       </c>
       <c r="AB43" s="7">
-        <f t="shared" si="48"/>
-        <v>0.10077155549171228</v>
+        <f t="shared" si="55"/>
+        <v>0.10186663611935132</v>
       </c>
       <c r="AC43" s="7">
-        <f t="shared" si="46"/>
-        <v>7.9000781194946093E-2</v>
+        <f t="shared" si="53"/>
+        <v>7.9364289942943922E-2</v>
       </c>
       <c r="AD43" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="53"/>
         <v>7.0957311657828981E-2</v>
       </c>
       <c r="AE43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>6.9149908436355975E-2</v>
       </c>
       <c r="AF43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>6.8293766712858223E-2</v>
       </c>
       <c r="AG43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>6.8096765462724973E-2</v>
       </c>
       <c r="AH43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>6.7900332485428636E-2</v>
       </c>
       <c r="AI43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>6.7704466141720654E-2</v>
       </c>
       <c r="AJ43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>6.7509164797081064E-2</v>
       </c>
       <c r="AK43" s="7">
-        <f t="shared" si="48"/>
+        <f t="shared" si="55"/>
         <v>6.7314426821704867E-2</v>
       </c>
     </row>
@@ -4742,111 +4819,111 @@
         <v>53</v>
       </c>
       <c r="C44" s="7">
-        <f t="shared" ref="C44:J44" si="49">C10/C$5</f>
+        <f t="shared" ref="C44:J44" si="57">C10/C$5</f>
         <v>2.032258064516129</v>
       </c>
       <c r="D44" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="57"/>
         <v>0.98768248175182471</v>
       </c>
       <c r="E44" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="57"/>
         <v>0.10889659722630504</v>
       </c>
       <c r="F44" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="57"/>
         <v>7.3243239361778525E-2</v>
       </c>
       <c r="G44" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="57"/>
         <v>7.5707675949076084E-2</v>
       </c>
       <c r="H44" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="57"/>
         <v>5.1550212602510803E-2</v>
       </c>
       <c r="I44" s="7">
-        <f t="shared" si="49"/>
+        <f t="shared" si="57"/>
         <v>4.7545651501083259E-2</v>
       </c>
-      <c r="J44" s="7" t="e">
-        <f t="shared" si="49"/>
-        <v>#DIV/0!</v>
+      <c r="J44" s="7">
+        <f t="shared" si="57"/>
+        <v>5.6792351852692977E-2</v>
       </c>
       <c r="S44" s="7">
-        <f t="shared" ref="S44:AK44" si="50">S10/S$5</f>
+        <f t="shared" ref="S44:AK44" si="58">S10/S$5</f>
         <v>5.3821643825098853E-2</v>
       </c>
       <c r="T44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>4.1343609186773149E-2</v>
       </c>
       <c r="U44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>4.1031078169537952E-2</v>
       </c>
       <c r="V44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>3.6758815271928723E-2</v>
       </c>
       <c r="W44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>3.5677274502631251E-2</v>
       </c>
       <c r="X44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>3.4445513881882529E-2</v>
       </c>
       <c r="Y44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>5.1097342781914357E-2</v>
       </c>
       <c r="Z44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>9.7224922914525405E-2</v>
       </c>
       <c r="AA44" s="7">
-        <f t="shared" si="50"/>
-        <v>5.1483488244378144E-2</v>
+        <f t="shared" ref="AA44" si="59">AA10/AA$5</f>
+        <v>5.4461823046558874E-2</v>
       </c>
       <c r="AB44" s="7">
-        <f t="shared" si="50"/>
-        <v>4.6020171690535308E-2</v>
+        <f t="shared" si="58"/>
+        <v>4.7320521099186899E-2</v>
       </c>
       <c r="AC44" s="7">
-        <f t="shared" si="46"/>
-        <v>4.2172581930137648E-2</v>
+        <f t="shared" si="53"/>
+        <v>4.2366631941104384E-2</v>
       </c>
       <c r="AD44" s="7">
-        <f t="shared" si="46"/>
+        <f t="shared" si="53"/>
         <v>3.7878777831927814E-2</v>
       </c>
       <c r="AE44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>3.6842471645959975E-2</v>
       </c>
       <c r="AF44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>3.6175798349509264E-2</v>
       </c>
       <c r="AG44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>3.5862738556100046E-2</v>
       </c>
       <c r="AH44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>3.555238793397994E-2</v>
       </c>
       <c r="AI44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>3.5244723038397416E-2</v>
       </c>
       <c r="AJ44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>3.4939720627488201E-2</v>
       </c>
       <c r="AK44" s="7">
-        <f t="shared" si="50"/>
+        <f t="shared" si="58"/>
         <v>3.4637357660519549E-2</v>
       </c>
     </row>
@@ -4859,68 +4936,68 @@
         <v>65.548387096774192</v>
       </c>
       <c r="D46" s="7">
-        <f t="shared" ref="D46:J46" si="51">D14/D5</f>
+        <f t="shared" ref="D46:J46" si="60">D14/D5</f>
         <v>42.309078467153284</v>
       </c>
       <c r="E46" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="60"/>
         <v>1.4968546063848551</v>
       </c>
       <c r="F46" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="60"/>
         <v>0.56138173268474434</v>
       </c>
       <c r="G46" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="60"/>
         <v>0.56749528216033951</v>
       </c>
       <c r="H46" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="60"/>
         <v>0.27719189482408907</v>
       </c>
       <c r="I46" s="7">
-        <f t="shared" si="51"/>
+        <f t="shared" si="60"/>
         <v>0.23230578768183227</v>
       </c>
-      <c r="J46" s="7" t="e">
-        <f t="shared" si="51"/>
-        <v>#DIV/0!</v>
+      <c r="J46" s="7">
+        <f t="shared" si="60"/>
+        <v>0.24917698683376421</v>
       </c>
       <c r="S46" s="7">
-        <f t="shared" ref="S46:AA46" si="52">S14/S5</f>
+        <f t="shared" ref="S46:Z46" si="61">S14/S5</f>
         <v>0.12897807977273601</v>
       </c>
       <c r="T46" s="7">
-        <f t="shared" si="52"/>
+        <f t="shared" si="61"/>
         <v>0.12773088047082293</v>
       </c>
       <c r="U46" s="7">
-        <f t="shared" si="52"/>
+        <f t="shared" si="61"/>
         <v>0.13666549454553362</v>
       </c>
       <c r="V46" s="7">
-        <f t="shared" si="52"/>
+        <f t="shared" si="61"/>
         <v>0.14338953054710049</v>
       </c>
       <c r="W46" s="7">
-        <f t="shared" si="52"/>
+        <f t="shared" si="61"/>
         <v>0.14829264184082383</v>
       </c>
       <c r="X46" s="7">
-        <f t="shared" si="52"/>
+        <f t="shared" si="61"/>
         <v>0.15084999644093974</v>
       </c>
       <c r="Y46" s="7">
-        <f t="shared" si="52"/>
+        <f t="shared" si="61"/>
         <v>0.5823065684305927</v>
       </c>
       <c r="Z46" s="7">
-        <f t="shared" si="52"/>
+        <f t="shared" si="61"/>
         <v>1.3757326592405346</v>
       </c>
       <c r="AA46" s="7">
-        <f t="shared" si="52"/>
-        <v>0.27850729947914499</v>
+        <f t="shared" ref="AA46" si="62">AA14/AA5</f>
+        <v>0.28471786380828118</v>
       </c>
       <c r="AB46" s="7">
         <v>0.2</v>
@@ -4962,23 +5039,23 @@
         <v>3.1673734341245187E-2</v>
       </c>
       <c r="T48" s="8">
-        <f t="shared" ref="T48:AK48" si="53">T15/T31</f>
+        <f t="shared" ref="T48:AK48" si="63">T15/T31</f>
         <v>4.5683807671163361E-2</v>
       </c>
       <c r="U48" s="8">
-        <f t="shared" si="53"/>
+        <f t="shared" si="63"/>
         <v>4.2746869347776668E-2</v>
       </c>
       <c r="V48" s="8">
-        <f t="shared" si="53"/>
+        <f t="shared" si="63"/>
         <v>4.6189715527067285E-2</v>
       </c>
       <c r="W48" s="8">
-        <f t="shared" si="53"/>
+        <f t="shared" si="63"/>
         <v>4.6294932534208168E-2</v>
       </c>
       <c r="X48" s="8">
-        <f t="shared" si="53"/>
+        <f t="shared" si="63"/>
         <v>4.9195566460835019E-2</v>
       </c>
       <c r="Y48" s="8">
@@ -4986,51 +5063,51 @@
         <v>6.0374014411877772E-2</v>
       </c>
       <c r="Z48" s="8">
-        <f t="shared" si="53"/>
+        <f t="shared" si="63"/>
         <v>5.1803929395068303E-2</v>
       </c>
-      <c r="AA48" s="8" t="e">
-        <f t="shared" si="53"/>
+      <c r="AA48" s="8">
+        <f t="shared" ref="AA48" si="64">AA15/AA31</f>
+        <v>5.1619668448701285E-2</v>
+      </c>
+      <c r="AB48" s="8" t="e">
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AB48" s="8" t="e">
-        <f t="shared" si="53"/>
+      <c r="AC48" s="8" t="e">
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC48" s="8" t="e">
-        <f t="shared" si="53"/>
+      <c r="AD48" s="8" t="e">
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD48" s="8" t="e">
-        <f t="shared" si="53"/>
+      <c r="AE48" s="8" t="e">
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE48" s="8" t="e">
-        <f t="shared" si="53"/>
+      <c r="AF48" s="8" t="e">
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AF48" s="8" t="e">
-        <f t="shared" si="53"/>
+      <c r="AG48" s="8" t="e">
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AG48" s="8" t="e">
-        <f t="shared" si="53"/>
+      <c r="AH48" s="8" t="e">
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH48" s="8" t="e">
-        <f t="shared" si="53"/>
+      <c r="AI48" s="8" t="e">
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AI48" s="8" t="e">
-        <f t="shared" si="53"/>
+      <c r="AJ48" s="8" t="e">
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AJ48" s="8" t="e">
-        <f t="shared" si="53"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="AK48" s="8" t="e">
-        <f t="shared" si="53"/>
+        <f t="shared" si="63"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -5043,36 +5120,36 @@
         <v>8.7382433106837104E-2</v>
       </c>
       <c r="T49" s="8">
-        <f t="shared" ref="T49:AA49" si="54">T15/T5</f>
+        <f t="shared" ref="T49:Z49" si="65">T15/T5</f>
         <v>9.9449192223007521E-2</v>
       </c>
       <c r="U49" s="8">
-        <f t="shared" si="54"/>
+        <f t="shared" si="65"/>
         <v>8.8729706541625819E-2</v>
       </c>
       <c r="V49" s="8">
-        <f t="shared" si="54"/>
+        <f t="shared" si="65"/>
         <v>9.4503421404976667E-2</v>
       </c>
       <c r="W49" s="8">
-        <f t="shared" si="54"/>
+        <f t="shared" si="65"/>
         <v>9.2658851235690814E-2</v>
       </c>
       <c r="X49" s="8">
-        <f t="shared" si="54"/>
+        <f t="shared" si="65"/>
         <v>9.9994119813443361E-2</v>
       </c>
       <c r="Y49" s="8">
-        <f t="shared" si="54"/>
+        <f t="shared" si="65"/>
         <v>0.56082068270425256</v>
       </c>
       <c r="Z49" s="8">
-        <f t="shared" si="54"/>
+        <f t="shared" si="65"/>
         <v>1.0815809698417549</v>
       </c>
       <c r="AA49" s="8">
-        <f t="shared" si="54"/>
-        <v>0.14853323190585219</v>
+        <f t="shared" ref="AA49" si="66">AA15/AA5</f>
+        <v>0.15470006771598924</v>
       </c>
       <c r="AB49" s="8">
         <v>0.13</v>
@@ -5110,36 +5187,36 @@
         <v>54</v>
       </c>
       <c r="T51" s="8">
-        <f t="shared" ref="T51:AA51" si="55">T18/S32</f>
+        <f t="shared" ref="T51:AA51" si="67">T18/S32</f>
         <v>3.6393879858209841E-2</v>
       </c>
       <c r="U51" s="8">
-        <f t="shared" si="55"/>
+        <f t="shared" si="67"/>
         <v>4.3715437999950424E-2</v>
       </c>
       <c r="V51" s="8">
-        <f t="shared" si="55"/>
+        <f t="shared" si="67"/>
         <v>4.2452332196109721E-2</v>
       </c>
       <c r="W51" s="8">
-        <f t="shared" si="55"/>
+        <f t="shared" si="67"/>
         <v>4.3718370268403951E-2</v>
       </c>
       <c r="X51" s="8">
-        <f t="shared" si="55"/>
+        <f t="shared" si="67"/>
         <v>4.2058044654737836E-2</v>
       </c>
       <c r="Y51" s="8">
-        <f t="shared" si="55"/>
+        <f t="shared" si="67"/>
         <v>7.2530743982264181E-2</v>
       </c>
       <c r="Z51" s="8">
-        <f t="shared" si="55"/>
+        <f t="shared" si="67"/>
         <v>0.24135432970753151</v>
       </c>
       <c r="AA51" s="8">
-        <f t="shared" si="55"/>
-        <v>7.1044209582782639E-2</v>
+        <f t="shared" si="67"/>
+        <v>7.3310253678034218E-2</v>
       </c>
       <c r="AB51" s="8">
         <v>7.0000000000000007E-2</v>
@@ -5181,36 +5258,36 @@
         <v>6.6613579532265087E-3</v>
       </c>
       <c r="T52" s="8">
-        <f t="shared" ref="T52:AA52" si="56">T21/T20</f>
+        <f t="shared" ref="T52:Z52" si="68">T21/T20</f>
         <v>-1.5602313843884667E-2</v>
       </c>
       <c r="U52" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="68"/>
         <v>-1.1243341833507961E-2</v>
       </c>
       <c r="V52" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="68"/>
         <v>-1.3939497752447389E-2</v>
       </c>
       <c r="W52" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="68"/>
         <v>-1.49594032745618E-2</v>
       </c>
       <c r="X52" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="68"/>
         <v>2.0696209060242887E-2</v>
       </c>
       <c r="Y52" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="68"/>
         <v>3.1250078125195316E-3</v>
       </c>
       <c r="Z52" s="8">
-        <f t="shared" si="56"/>
+        <f t="shared" si="68"/>
         <v>1.1701025144874332E-3</v>
       </c>
       <c r="AA52" s="8">
-        <f t="shared" si="56"/>
-        <v>-8.5142640221531792E-3</v>
+        <f t="shared" ref="AA52" si="69">AA21/AA20</f>
+        <v>-2.9867843576832382E-3</v>
       </c>
       <c r="AB52" s="8">
         <v>0.01</v>
@@ -5361,27 +5438,27 @@
         <v>2.4495528999999996</v>
       </c>
       <c r="AF57" s="2">
-        <f t="shared" ref="AF57:AK57" si="57">AE57*(1+AF58)</f>
+        <f t="shared" ref="AF57:AK57" si="70">AE57*(1+AF58)</f>
         <v>2.5401863572999992</v>
       </c>
       <c r="AG57" s="2">
-        <f t="shared" si="57"/>
+        <f t="shared" si="70"/>
         <v>2.6341732525200992</v>
       </c>
       <c r="AH57" s="2">
-        <f t="shared" si="57"/>
+        <f t="shared" si="70"/>
         <v>2.7316376628633425</v>
       </c>
       <c r="AI57" s="2">
-        <f t="shared" si="57"/>
+        <f t="shared" si="70"/>
         <v>2.832708256389286</v>
       </c>
       <c r="AJ57" s="2">
-        <f t="shared" si="57"/>
+        <f t="shared" si="70"/>
         <v>2.9375184618756895</v>
       </c>
       <c r="AK57" s="2">
-        <f t="shared" si="57"/>
+        <f t="shared" si="70"/>
         <v>3.04620664496509</v>
       </c>
     </row>
@@ -5397,27 +5474,27 @@
         <v>2.941176470588247E-2</v>
       </c>
       <c r="X58" s="9">
-        <f t="shared" ref="X58:AC58" si="58">X57/W57-1</f>
+        <f t="shared" ref="X58:AC58" si="71">X57/W57-1</f>
         <v>-2.8571428571428581E-2</v>
       </c>
       <c r="Y58" s="9">
-        <f t="shared" si="58"/>
+        <f t="shared" si="71"/>
         <v>-0.26470588235294112</v>
       </c>
       <c r="Z58" s="9">
-        <f t="shared" si="58"/>
+        <f t="shared" si="71"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="AA58" s="9">
-        <f t="shared" si="58"/>
+        <f t="shared" si="71"/>
         <v>0.42500000000000004</v>
       </c>
       <c r="AB58" s="9">
-        <f t="shared" si="58"/>
+        <f t="shared" si="71"/>
         <v>-0.1228070175438597</v>
       </c>
       <c r="AC58" s="9">
-        <f t="shared" si="58"/>
+        <f t="shared" si="71"/>
         <v>-8.0000000000000071E-2</v>
       </c>
       <c r="AD58" s="9">
@@ -5589,9 +5666,9 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="66" spans="2:27" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E66" s="24">
         <v>0.40265600000000001</v>
@@ -5608,6 +5685,9 @@
       <c r="I66" s="24">
         <v>3.9825590000000002</v>
       </c>
+      <c r="J66" s="24">
+        <v>4.3804999999999996</v>
+      </c>
       <c r="O66" s="24">
         <v>9.5589999999999993</v>
       </c>
@@ -5645,13 +5725,12 @@
         <v>1.7788999999999999</v>
       </c>
       <c r="AA66" s="24">
-        <f>G66+H66+I66+I66</f>
-        <v>12.393864000000001</v>
-      </c>
-    </row>
-    <row r="67" spans="2:27" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>12.79177</v>
+      </c>
+    </row>
+    <row r="67" spans="2:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E67" s="24">
         <v>0.70135000000000003</v>
@@ -5668,6 +5747,9 @@
       <c r="I67" s="24">
         <v>4.8874149999999998</v>
       </c>
+      <c r="J67" s="24">
+        <v>5.0609000000000002</v>
+      </c>
       <c r="O67" s="24">
         <v>8.7909799999999994</v>
       </c>
@@ -5705,265 +5787,283 @@
         <v>3.3767</v>
       </c>
       <c r="AA67" s="24">
-        <f>G67+H67+I67+I67</f>
-        <v>17.392282999999999</v>
-      </c>
-    </row>
-    <row r="68" spans="2:27" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="2:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>17.565999999999999</v>
+      </c>
+      <c r="AB67" s="24">
+        <v>22.8</v>
+      </c>
+    </row>
+    <row r="68" spans="2:28" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:28" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E69" s="8">
+        <f t="shared" ref="E69:J69" si="72">E66/E67</f>
+        <v>0.57411563413416977</v>
+      </c>
+      <c r="F69" s="8">
+        <f t="shared" si="72"/>
+        <v>0.51439998504868523</v>
+      </c>
+      <c r="G69" s="8">
+        <f t="shared" si="72"/>
+        <v>0.47994512403331641</v>
+      </c>
+      <c r="H69" s="8">
+        <f t="shared" si="72"/>
+        <v>0.64652626587053519</v>
+      </c>
+      <c r="I69" s="8">
+        <f t="shared" si="72"/>
+        <v>0.81486000268035363</v>
+      </c>
+      <c r="J69" s="8">
+        <f t="shared" si="72"/>
+        <v>0.86555750953387722</v>
+      </c>
+      <c r="O69" s="8">
+        <f t="shared" ref="O69:AA69" si="73">O66/O67</f>
+        <v>1.0873645486623789</v>
+      </c>
+      <c r="P69" s="8">
+        <f t="shared" si="73"/>
+        <v>1.0817071235919404</v>
+      </c>
+      <c r="Q69" s="8">
+        <f t="shared" si="73"/>
+        <v>1.0760411134368459</v>
+      </c>
+      <c r="R69" s="8">
+        <f t="shared" si="73"/>
+        <v>1.091392085160154</v>
+      </c>
+      <c r="S69" s="8">
+        <f t="shared" si="73"/>
+        <v>1.0896739130434783</v>
+      </c>
+      <c r="T69" s="8">
+        <f t="shared" si="73"/>
+        <v>1.0902721088435376</v>
+      </c>
+      <c r="U69" s="8">
+        <f t="shared" si="73"/>
+        <v>1.0740534929164629</v>
+      </c>
+      <c r="V69" s="8">
+        <f t="shared" si="73"/>
+        <v>1.0667841551769814</v>
+      </c>
+      <c r="W69" s="8">
+        <f t="shared" si="73"/>
+        <v>1.0761559527853259</v>
+      </c>
+      <c r="X69" s="8">
+        <f t="shared" si="73"/>
+        <v>1.0730212208418144</v>
+      </c>
+      <c r="Y69" s="8">
+        <f t="shared" si="73"/>
+        <v>1.0375381929288521</v>
+      </c>
+      <c r="Z69" s="8">
+        <f t="shared" si="73"/>
+        <v>0.52681612224953356</v>
+      </c>
+      <c r="AA69" s="8">
+        <f t="shared" si="73"/>
+        <v>0.72821188659911196</v>
+      </c>
+    </row>
+    <row r="70" spans="2:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E69" s="8">
-        <f>E66/E67</f>
-        <v>0.57411563413416977</v>
-      </c>
-      <c r="F69" s="8">
-        <f>F66/F67</f>
-        <v>0.51439998504868523</v>
-      </c>
-      <c r="G69" s="8">
-        <f>G66/G67</f>
-        <v>0.47994512403331641</v>
-      </c>
-      <c r="H69" s="8">
-        <f>H66/H67</f>
-        <v>0.64652626587053519</v>
-      </c>
-      <c r="I69" s="8">
-        <f>I66/I67</f>
-        <v>0.81486000268035363</v>
-      </c>
-      <c r="O69" s="8">
-        <f t="shared" ref="O69:AA69" si="59">O66/O67</f>
-        <v>1.0873645486623789</v>
-      </c>
-      <c r="P69" s="8">
-        <f t="shared" si="59"/>
-        <v>1.0817071235919404</v>
-      </c>
-      <c r="Q69" s="8">
-        <f t="shared" si="59"/>
-        <v>1.0760411134368459</v>
-      </c>
-      <c r="R69" s="8">
-        <f t="shared" si="59"/>
-        <v>1.091392085160154</v>
-      </c>
-      <c r="S69" s="8">
-        <f t="shared" si="59"/>
-        <v>1.0896739130434783</v>
-      </c>
-      <c r="T69" s="8">
-        <f t="shared" si="59"/>
-        <v>1.0902721088435376</v>
-      </c>
-      <c r="U69" s="8">
-        <f t="shared" si="59"/>
-        <v>1.0740534929164629</v>
-      </c>
-      <c r="V69" s="8">
-        <f t="shared" si="59"/>
-        <v>1.0667841551769814</v>
-      </c>
-      <c r="W69" s="8">
-        <f t="shared" si="59"/>
-        <v>1.0761559527853259</v>
-      </c>
-      <c r="X69" s="8">
-        <f t="shared" si="59"/>
-        <v>1.0730212208418144</v>
-      </c>
-      <c r="Y69" s="8">
-        <f t="shared" si="59"/>
-        <v>1.0375381929288521</v>
-      </c>
-      <c r="Z69" s="8">
-        <f t="shared" si="59"/>
-        <v>0.52681612224953356</v>
-      </c>
-      <c r="AA69" s="8">
-        <f t="shared" si="59"/>
-        <v>0.71260707981810101</v>
-      </c>
-    </row>
-    <row r="70" spans="2:27" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="24" t="s">
+      <c r="E70" s="24">
+        <f t="shared" ref="E70:J70" si="74">E5/E66</f>
+        <v>380.17811730112049</v>
+      </c>
+      <c r="F70" s="24">
+        <f t="shared" si="74"/>
+        <v>354.17599186164801</v>
+      </c>
+      <c r="G70" s="24">
+        <f t="shared" si="74"/>
+        <v>365.1449582565553</v>
+      </c>
+      <c r="H70" s="24">
+        <f t="shared" si="74"/>
+        <v>395.82302537258698</v>
+      </c>
+      <c r="I70" s="24">
+        <f t="shared" si="74"/>
+        <v>405.64370797770977</v>
+      </c>
+      <c r="J70" s="24">
+        <f t="shared" si="74"/>
+        <v>346.78986417075686</v>
+      </c>
+      <c r="O70" s="24">
+        <f t="shared" ref="O70:AA70" si="75">O5/O66</f>
+        <v>210.49272936499634</v>
+      </c>
+      <c r="P70" s="24">
+        <f t="shared" si="75"/>
+        <v>217.00625794465634</v>
+      </c>
+      <c r="Q70" s="24">
+        <f t="shared" si="75"/>
+        <v>220.29633500759709</v>
+      </c>
+      <c r="R70" s="24">
+        <f t="shared" si="75"/>
+        <v>225.44886807181891</v>
+      </c>
+      <c r="S70" s="24">
+        <f t="shared" si="75"/>
+        <v>229.27094029631803</v>
+      </c>
+      <c r="T70" s="24">
+        <f t="shared" si="75"/>
+        <v>271.10956510887877</v>
+      </c>
+      <c r="U70" s="24">
+        <f t="shared" si="75"/>
+        <v>277.12986178626051</v>
+      </c>
+      <c r="V70" s="24">
+        <f t="shared" si="75"/>
+        <v>291.32294984613725</v>
+      </c>
+      <c r="W70" s="24">
+        <f t="shared" si="75"/>
+        <v>298.62722856508765</v>
+      </c>
+      <c r="X70" s="24">
+        <f t="shared" si="75"/>
+        <v>313.13166552798492</v>
+      </c>
+      <c r="Y70" s="24">
+        <f t="shared" si="75"/>
+        <v>299.1422427896976</v>
+      </c>
+      <c r="Z70" s="24">
+        <f t="shared" si="75"/>
+        <v>364.25993591545335</v>
+      </c>
+      <c r="AA70" s="24">
+        <f t="shared" si="75"/>
+        <v>378.66221797296231</v>
+      </c>
+    </row>
+    <row r="71" spans="2:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="E70" s="24">
-        <f>E5/E66</f>
-        <v>380.17811730112049</v>
-      </c>
-      <c r="F70" s="24">
-        <f>F5/F66</f>
-        <v>354.17599186164801</v>
-      </c>
-      <c r="G70" s="24">
-        <f>G5/G66</f>
-        <v>365.1449582565553</v>
-      </c>
-      <c r="H70" s="24">
-        <f>H5/H66</f>
-        <v>395.82302537258698</v>
-      </c>
-      <c r="I70" s="24">
-        <f>I5/I66</f>
-        <v>405.64370797770977</v>
-      </c>
-      <c r="O70" s="24">
-        <f t="shared" ref="O70:AA70" si="60">O5/O66</f>
-        <v>210.49272936499634</v>
-      </c>
-      <c r="P70" s="24">
-        <f t="shared" si="60"/>
-        <v>217.00625794465634</v>
-      </c>
-      <c r="Q70" s="24">
-        <f t="shared" si="60"/>
-        <v>220.29633500759709</v>
-      </c>
-      <c r="R70" s="24">
-        <f t="shared" si="60"/>
-        <v>225.44886807181891</v>
-      </c>
-      <c r="S70" s="24">
-        <f t="shared" si="60"/>
-        <v>229.27094029631803</v>
-      </c>
-      <c r="T70" s="24">
-        <f t="shared" si="60"/>
-        <v>271.10956510887877</v>
-      </c>
-      <c r="U70" s="24">
-        <f t="shared" si="60"/>
-        <v>277.12986178626051</v>
-      </c>
-      <c r="V70" s="24">
-        <f t="shared" si="60"/>
-        <v>291.32294984613725</v>
-      </c>
-      <c r="W70" s="24">
-        <f t="shared" si="60"/>
-        <v>298.62722856508765</v>
-      </c>
-      <c r="X70" s="24">
-        <f t="shared" si="60"/>
-        <v>313.13166552798492</v>
-      </c>
-      <c r="Y70" s="24">
-        <f t="shared" si="60"/>
-        <v>299.1422427896976</v>
-      </c>
-      <c r="Z70" s="24">
-        <f t="shared" si="60"/>
-        <v>364.25993591545335</v>
-      </c>
-      <c r="AA70" s="24">
-        <f t="shared" si="60"/>
-        <v>398.59619243845185</v>
-      </c>
-    </row>
-    <row r="71" spans="2:27" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="24" t="s">
-        <v>78</v>
-      </c>
       <c r="E71" s="24">
-        <f>E5/E67</f>
+        <f t="shared" ref="E71:J71" si="76">E5/E67</f>
         <v>218.26620089826761</v>
       </c>
       <c r="F71" s="24">
-        <f>F5/F67</f>
+        <f t="shared" si="76"/>
         <v>182.18812491823502</v>
       </c>
       <c r="G71" s="24">
-        <f>G5/G67</f>
+        <f t="shared" si="76"/>
         <v>175.24954228058257</v>
       </c>
       <c r="H71" s="24">
-        <f>H5/H67</f>
+        <f t="shared" si="76"/>
         <v>255.90998253971676</v>
       </c>
       <c r="I71" s="24">
-        <f>I5/I67</f>
+        <f t="shared" si="76"/>
         <v>330.54283296998517</v>
       </c>
+      <c r="J71" s="24">
+        <f t="shared" si="76"/>
+        <v>300.16657116323188</v>
+      </c>
       <c r="O71" s="24">
-        <f t="shared" ref="O71:AA71" si="61">O5/O67</f>
+        <f t="shared" ref="O71:AA71" si="77">O5/O67</f>
         <v>228.88233166268154</v>
       </c>
       <c r="P71" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="77"/>
         <v>234.73721508276486</v>
       </c>
       <c r="Q71" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="77"/>
         <v>237.04791360763119</v>
       </c>
       <c r="R71" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="77"/>
         <v>246.05311022189892</v>
       </c>
       <c r="S71" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="77"/>
         <v>249.83056265984655</v>
       </c>
       <c r="T71" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="77"/>
         <v>295.5831972789116</v>
       </c>
       <c r="U71" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="77"/>
         <v>297.65229604298975</v>
       </c>
       <c r="V71" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="77"/>
         <v>310.77870693527768</v>
       </c>
       <c r="W71" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="77"/>
         <v>321.36946968410325</v>
       </c>
       <c r="X71" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="77"/>
         <v>335.99692202906908</v>
       </c>
       <c r="Y71" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="77"/>
         <v>310.37150201270674</v>
       </c>
       <c r="Z71" s="24">
-        <f t="shared" si="61"/>
+        <f t="shared" si="77"/>
         <v>191.89800692984272</v>
       </c>
       <c r="AA71" s="24">
-        <f t="shared" si="61"/>
-        <v>284.04246872017899</v>
-      </c>
-    </row>
-    <row r="73" spans="2:27" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="77"/>
+        <v>275.74632813389508</v>
+      </c>
+    </row>
+    <row r="73" spans="2:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E73" s="24">
-        <f>E3/E66</f>
+        <f t="shared" ref="E73:J73" si="78">E3/E66</f>
         <v>213.8972224429786</v>
       </c>
       <c r="F73" s="24">
-        <f>F3/F66</f>
+        <f t="shared" si="78"/>
         <v>221.53393402121785</v>
       </c>
       <c r="G73" s="24">
-        <f>G3/G66</f>
+        <f t="shared" si="78"/>
         <v>239.57183412314978</v>
       </c>
       <c r="H73" s="24">
-        <f>H3/H66</f>
+        <f t="shared" si="78"/>
         <v>264.69242823325447</v>
       </c>
       <c r="I73" s="24">
-        <f>I3/I66</f>
+        <f t="shared" si="78"/>
         <v>277.68577941971483</v>
+      </c>
+      <c r="J73" s="24">
+        <f t="shared" si="78"/>
+        <v>230.92181257847281</v>
       </c>
       <c r="O73" s="24">
         <f>O3/O66</f>
@@ -5982,19 +6082,19 @@
         <v>159.27689919216905</v>
       </c>
       <c r="S73" s="24">
-        <f t="shared" ref="S73:Z73" si="62">S3/S66</f>
+        <f t="shared" ref="S73:Z73" si="79">S3/S66</f>
         <v>159.61199941323164</v>
       </c>
       <c r="T73" s="24">
-        <f t="shared" si="62"/>
+        <f t="shared" si="79"/>
         <v>195.23928370874148</v>
       </c>
       <c r="U73" s="24">
-        <f t="shared" si="62"/>
+        <f t="shared" si="79"/>
         <v>192.67791252338151</v>
       </c>
       <c r="V73" s="24">
-        <f t="shared" si="62"/>
+        <f t="shared" si="79"/>
         <v>202.45262646439562</v>
       </c>
       <c r="W73" s="24">
@@ -6002,100 +6102,104 @@
         <v>210.08630680837422</v>
       </c>
       <c r="X73" s="24">
-        <f t="shared" si="62"/>
+        <f t="shared" si="79"/>
         <v>218.8885497070923</v>
       </c>
       <c r="Y73" s="24">
-        <f t="shared" si="62"/>
+        <f t="shared" si="79"/>
         <v>202.66208572897676</v>
       </c>
       <c r="Z73" s="24">
-        <f t="shared" si="62"/>
+        <f t="shared" si="79"/>
         <v>220.78363033335208</v>
       </c>
       <c r="AA73" s="24">
         <f>AA3/AA66</f>
-        <v>270.1455333058359</v>
-      </c>
-    </row>
-    <row r="74" spans="2:27" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <v>254.3666748229526</v>
+      </c>
+    </row>
+    <row r="74" spans="2:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E74" s="24">
         <f>E4/E66</f>
         <v>166.28089485814192</v>
       </c>
       <c r="F74" s="24">
-        <f t="shared" ref="F74:I74" si="63">F4/F66</f>
+        <f t="shared" ref="F74:I74" si="80">F4/F66</f>
         <v>132.64205784043017</v>
       </c>
       <c r="G74" s="24">
-        <f t="shared" si="63"/>
+        <f t="shared" si="80"/>
         <v>125.57312413340553</v>
       </c>
       <c r="H74" s="24">
-        <f t="shared" si="63"/>
+        <f t="shared" si="80"/>
         <v>131.13059713933251</v>
       </c>
       <c r="I74" s="24">
-        <f t="shared" si="63"/>
+        <f t="shared" si="80"/>
         <v>127.957928557995</v>
       </c>
+      <c r="J74" s="24">
+        <f t="shared" ref="J74" si="81">J4/J66</f>
+        <v>115.86805159228403</v>
+      </c>
       <c r="O74" s="24">
-        <f t="shared" ref="O74:AA74" si="64">O4/O66</f>
+        <f t="shared" ref="O74:AA74" si="82">O4/O66</f>
         <v>62.799456010042888</v>
       </c>
       <c r="P74" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>64.140021511684765</v>
       </c>
       <c r="Q74" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>65.005951862497454</v>
       </c>
       <c r="R74" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>66.171968879649853</v>
       </c>
       <c r="S74" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>69.658940883086402</v>
       </c>
       <c r="T74" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>75.870281400137259</v>
       </c>
       <c r="U74" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>84.451949262879012</v>
       </c>
       <c r="V74" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>88.870323381741613</v>
       </c>
       <c r="W74" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>88.540921756713445</v>
       </c>
       <c r="X74" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>94.24311582089264</v>
       </c>
       <c r="Y74" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>96.480157060720799</v>
       </c>
       <c r="Z74" s="24">
-        <f t="shared" si="64"/>
+        <f t="shared" si="82"/>
         <v>143.4763055821013</v>
       </c>
       <c r="AA74" s="24">
-        <f t="shared" si="64"/>
-        <v>128.45065913261593</v>
-      </c>
-    </row>
-    <row r="75" spans="2:27" x14ac:dyDescent="0.25">
+        <f t="shared" si="82"/>
+        <v>124.29554315000973</v>
+      </c>
+    </row>
+    <row r="75" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B75" s="24"/>
       <c r="C75" s="24"/>
       <c r="D75" s="24"/>
@@ -6123,161 +6227,169 @@
       <c r="Z75" s="24"/>
       <c r="AA75" s="24"/>
     </row>
-    <row r="76" spans="2:27" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E76" s="24">
         <f>E3/E$67</f>
         <v>122.80173950238824</v>
       </c>
       <c r="F76" s="24">
-        <f t="shared" ref="F76:I76" si="65">F3/F$67</f>
+        <f t="shared" ref="F76:I76" si="83">F3/F$67</f>
         <v>113.95705234829089</v>
       </c>
       <c r="G76" s="24">
-        <f t="shared" si="65"/>
+        <f t="shared" si="83"/>
         <v>114.98133364312424</v>
       </c>
       <c r="H76" s="24">
-        <f t="shared" si="65"/>
+        <f t="shared" si="83"/>
         <v>171.13060722985063</v>
       </c>
       <c r="I76" s="24">
-        <f t="shared" si="65"/>
+        <f t="shared" si="83"/>
         <v>226.27503496224489</v>
       </c>
+      <c r="J76" s="24">
+        <f t="shared" ref="J76" si="84">J3/J$67</f>
+        <v>199.8761089924717</v>
+      </c>
       <c r="O76" s="24">
-        <f t="shared" ref="O76:AA76" si="66">O3/O$67</f>
+        <f t="shared" ref="O76:AA76" si="85">O3/O$67</f>
         <v>160.59642952207832</v>
       </c>
       <c r="P76" s="24">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>165.35649690623515</v>
       </c>
       <c r="Q76" s="24">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>167.09883678548741</v>
       </c>
       <c r="R76" s="24">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>173.83354712718503</v>
       </c>
       <c r="S76" s="24">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>173.92503196930946</v>
       </c>
       <c r="T76" s="24">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>212.8639455782313</v>
       </c>
       <c r="U76" s="24">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>206.94638495359061</v>
       </c>
       <c r="V76" s="24">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>215.9732540861813</v>
       </c>
       <c r="W76" s="24">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>226.08562967051628</v>
       </c>
       <c r="X76" s="24">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>234.87205883499837</v>
       </c>
       <c r="Y76" s="24">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>210.26965420243465</v>
       </c>
       <c r="Z76" s="24">
-        <f t="shared" si="66"/>
+        <f t="shared" si="85"/>
         <v>116.31237598839104</v>
       </c>
       <c r="AA76" s="24">
-        <f t="shared" si="66"/>
-        <v>192.50761961497525</v>
-      </c>
-    </row>
-    <row r="77" spans="2:27" s="24" customFormat="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="85"/>
+        <v>185.23283616076515</v>
+      </c>
+    </row>
+    <row r="77" spans="2:28" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E77" s="24">
         <f>E4/E$67</f>
         <v>95.464461395879368</v>
       </c>
       <c r="F77" s="24">
-        <f t="shared" ref="F77:I77" si="67">F4/F$67</f>
+        <f t="shared" ref="F77:I77" si="86">F4/F$67</f>
         <v>68.231072569944118</v>
       </c>
       <c r="G77" s="24">
-        <f t="shared" si="67"/>
+        <f t="shared" si="86"/>
         <v>60.268208637458358</v>
       </c>
       <c r="H77" s="24">
-        <f t="shared" si="67"/>
+        <f t="shared" si="86"/>
         <v>84.77937530986614</v>
       </c>
       <c r="I77" s="24">
-        <f t="shared" si="67"/>
+        <f t="shared" si="86"/>
         <v>104.2677980077403</v>
       </c>
+      <c r="J77" s="24">
+        <f t="shared" ref="J77" si="87">J4/J$67</f>
+        <v>100.29046217076018</v>
+      </c>
       <c r="O77" s="24">
-        <f t="shared" ref="O77:AA77" si="68">O4/O$67</f>
+        <f t="shared" ref="O77:AA77" si="88">O4/O$67</f>
         <v>68.285902140603213</v>
       </c>
       <c r="P77" s="24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="88"/>
         <v>69.380718176529697</v>
       </c>
       <c r="Q77" s="24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="88"/>
         <v>69.94907682214378</v>
       </c>
       <c r="R77" s="24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="88"/>
         <v>72.219563094713862</v>
       </c>
       <c r="S77" s="24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="88"/>
         <v>75.905530690537077</v>
       </c>
       <c r="T77" s="24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="88"/>
         <v>82.719251700680275</v>
       </c>
       <c r="U77" s="24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="88"/>
         <v>90.705911089399123</v>
       </c>
       <c r="V77" s="24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="88"/>
         <v>94.805452849096383</v>
       </c>
       <c r="W77" s="24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="88"/>
         <v>95.283840013586953</v>
       </c>
       <c r="X77" s="24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="88"/>
         <v>101.12486319407074</v>
       </c>
       <c r="Y77" s="24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="88"/>
         <v>100.10184781027208</v>
       </c>
       <c r="Z77" s="24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="88"/>
         <v>75.585630941451711</v>
       </c>
       <c r="AA77" s="24">
-        <f t="shared" si="68"/>
-        <v>91.534849105203733</v>
-      </c>
-    </row>
-    <row r="78" spans="2:27" x14ac:dyDescent="0.25">
+        <f t="shared" si="88"/>
+        <v>90.513491973129916</v>
+      </c>
+    </row>
+    <row r="78" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B78" s="24"/>
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
@@ -6305,7 +6417,7 @@
       <c r="Z78" s="7"/>
       <c r="AA78" s="7"/>
     </row>
-    <row r="79" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B79" s="24"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
@@ -6412,7 +6524,7 @@
       </c>
       <c r="C4" s="4">
         <f>NPV(C3,Model!AB22:DX22)</f>
-        <v>9576.3280554549001</v>
+        <v>9564.1035156825055</v>
       </c>
     </row>
   </sheetData>

</xml_diff>